<commit_message>
fix bug kdr001-update template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
@@ -1559,9 +1559,6 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1667,6 +1664,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1691,11 +1694,8 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1742,7 +1742,7 @@
         <xdr:cNvPr id="2" name="楕円 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2230,29 +2230,29 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="12" customHeight="1">
-      <c r="A2" s="172"/>
-      <c r="B2" s="172"/>
-      <c r="C2" s="172"/>
-      <c r="D2" s="172"/>
-      <c r="E2" s="172"/>
-      <c r="F2" s="172"/>
-      <c r="G2" s="172"/>
-      <c r="H2" s="172"/>
-      <c r="I2" s="172"/>
-      <c r="J2" s="172"/>
-      <c r="K2" s="172"/>
-      <c r="L2" s="172"/>
-      <c r="M2" s="172"/>
-      <c r="N2" s="172"/>
-      <c r="O2" s="172"/>
-      <c r="P2" s="172"/>
-      <c r="Q2" s="172"/>
-      <c r="R2" s="172"/>
-      <c r="S2" s="172"/>
-      <c r="T2" s="172"/>
-      <c r="U2" s="172"/>
-      <c r="V2" s="172"/>
-      <c r="W2" s="172"/>
+      <c r="A2" s="173"/>
+      <c r="B2" s="173"/>
+      <c r="C2" s="173"/>
+      <c r="D2" s="173"/>
+      <c r="E2" s="173"/>
+      <c r="F2" s="173"/>
+      <c r="G2" s="173"/>
+      <c r="H2" s="173"/>
+      <c r="I2" s="173"/>
+      <c r="J2" s="173"/>
+      <c r="K2" s="173"/>
+      <c r="L2" s="173"/>
+      <c r="M2" s="173"/>
+      <c r="N2" s="173"/>
+      <c r="O2" s="173"/>
+      <c r="P2" s="173"/>
+      <c r="Q2" s="173"/>
+      <c r="R2" s="173"/>
+      <c r="S2" s="173"/>
+      <c r="T2" s="173"/>
+      <c r="U2" s="173"/>
+      <c r="V2" s="173"/>
+      <c r="W2" s="173"/>
     </row>
     <row r="3" spans="1:23" ht="12" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
@@ -2284,13 +2284,13 @@
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="173"/>
-      <c r="F4" s="174"/>
-      <c r="G4" s="174"/>
-      <c r="H4" s="174"/>
-      <c r="I4" s="175"/>
-      <c r="J4" s="176"/>
-      <c r="K4" s="177"/>
+      <c r="E4" s="174"/>
+      <c r="F4" s="175"/>
+      <c r="G4" s="175"/>
+      <c r="H4" s="175"/>
+      <c r="I4" s="176"/>
+      <c r="J4" s="177"/>
+      <c r="K4" s="178"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -2330,33 +2330,33 @@
       <c r="W5" s="131"/>
     </row>
     <row r="6" spans="1:23" ht="12" customHeight="1" thickBot="1">
-      <c r="A6" s="178"/>
-      <c r="B6" s="178"/>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178"/>
-      <c r="E6" s="178"/>
-      <c r="F6" s="178"/>
-      <c r="G6" s="178"/>
-      <c r="H6" s="178"/>
-      <c r="I6" s="178"/>
-      <c r="J6" s="178"/>
-      <c r="K6" s="178"/>
-      <c r="L6" s="178"/>
-      <c r="M6" s="178"/>
-      <c r="N6" s="178"/>
-      <c r="O6" s="178"/>
-      <c r="P6" s="178"/>
-      <c r="Q6" s="178"/>
-      <c r="R6" s="178"/>
-      <c r="S6" s="178"/>
-      <c r="T6" s="178"/>
-      <c r="U6" s="178"/>
-      <c r="V6" s="178"/>
-      <c r="W6" s="178"/>
+      <c r="A6" s="179"/>
+      <c r="B6" s="179"/>
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
+      <c r="G6" s="179"/>
+      <c r="H6" s="179"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="179"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="179"/>
+      <c r="M6" s="179"/>
+      <c r="N6" s="179"/>
+      <c r="O6" s="179"/>
+      <c r="P6" s="179"/>
+      <c r="Q6" s="179"/>
+      <c r="R6" s="179"/>
+      <c r="S6" s="179"/>
+      <c r="T6" s="179"/>
+      <c r="U6" s="179"/>
+      <c r="V6" s="179"/>
+      <c r="W6" s="179"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
-      <c r="A7" s="179"/>
-      <c r="B7" s="179"/>
+      <c r="A7" s="180"/>
+      <c r="B7" s="180"/>
       <c r="C7" s="10"/>
       <c r="D7" s="11"/>
       <c r="E7" s="12"/>
@@ -2364,24 +2364,24 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
       <c r="I7" s="68"/>
-      <c r="J7" s="142"/>
-      <c r="K7" s="143"/>
-      <c r="L7" s="144"/>
-      <c r="M7" s="144"/>
-      <c r="N7" s="144"/>
-      <c r="O7" s="144"/>
-      <c r="P7" s="144"/>
-      <c r="Q7" s="144"/>
-      <c r="R7" s="144"/>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="144"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="145"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="142"/>
+      <c r="L7" s="143"/>
+      <c r="M7" s="143"/>
+      <c r="N7" s="143"/>
+      <c r="O7" s="143"/>
+      <c r="P7" s="143"/>
+      <c r="Q7" s="143"/>
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
+      <c r="T7" s="143"/>
+      <c r="U7" s="143"/>
+      <c r="V7" s="143"/>
+      <c r="W7" s="144"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="180"/>
-      <c r="B8" s="180"/>
+      <c r="A8" s="171"/>
+      <c r="B8" s="171"/>
       <c r="C8" s="14"/>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
@@ -2405,8 +2405,8 @@
       <c r="W8" s="132"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
-      <c r="A9" s="181"/>
-      <c r="B9" s="181"/>
+      <c r="A9" s="172"/>
+      <c r="B9" s="172"/>
       <c r="C9" s="14"/>
       <c r="D9" s="19"/>
       <c r="E9" s="20"/>
@@ -2414,24 +2414,24 @@
       <c r="G9" s="22"/>
       <c r="H9" s="23"/>
       <c r="I9" s="69"/>
-      <c r="J9" s="146"/>
-      <c r="K9" s="147"/>
-      <c r="L9" s="148"/>
-      <c r="M9" s="148"/>
-      <c r="N9" s="148"/>
-      <c r="O9" s="148"/>
-      <c r="P9" s="148"/>
-      <c r="Q9" s="148"/>
-      <c r="R9" s="148"/>
-      <c r="S9" s="148"/>
-      <c r="T9" s="148"/>
-      <c r="U9" s="148"/>
-      <c r="V9" s="140"/>
-      <c r="W9" s="133"/>
+      <c r="J9" s="145"/>
+      <c r="K9" s="146"/>
+      <c r="L9" s="147"/>
+      <c r="M9" s="147"/>
+      <c r="N9" s="147"/>
+      <c r="O9" s="147"/>
+      <c r="P9" s="147"/>
+      <c r="Q9" s="147"/>
+      <c r="R9" s="147"/>
+      <c r="S9" s="147"/>
+      <c r="T9" s="147"/>
+      <c r="U9" s="147"/>
+      <c r="V9" s="139"/>
+      <c r="W9" s="157"/>
     </row>
     <row r="10" spans="1:23" ht="12" customHeight="1">
-      <c r="A10" s="180"/>
-      <c r="B10" s="180"/>
+      <c r="A10" s="171"/>
+      <c r="B10" s="171"/>
       <c r="C10" s="14"/>
       <c r="D10" s="24"/>
       <c r="E10" s="16"/>
@@ -2452,11 +2452,11 @@
       <c r="T10" s="73"/>
       <c r="U10" s="73"/>
       <c r="V10" s="73"/>
-      <c r="W10" s="134"/>
+      <c r="W10" s="132"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
-      <c r="A11" s="180"/>
-      <c r="B11" s="180"/>
+      <c r="A11" s="171"/>
+      <c r="B11" s="171"/>
       <c r="C11" s="14"/>
       <c r="D11" s="15"/>
       <c r="E11" s="25"/>
@@ -2507,8 +2507,8 @@
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="18"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="170"/>
-      <c r="D13" s="171"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
       <c r="E13" s="30"/>
       <c r="F13" s="31"/>
       <c r="G13" s="31"/>
@@ -2525,7 +2525,7 @@
       <c r="R13" s="55"/>
       <c r="S13" s="55"/>
       <c r="T13" s="55"/>
-      <c r="U13" s="141"/>
+      <c r="U13" s="140"/>
       <c r="V13" s="55"/>
       <c r="W13" s="135"/>
     </row>
@@ -2552,38 +2552,38 @@
       <c r="T14" s="86"/>
       <c r="U14" s="86"/>
       <c r="V14" s="86"/>
-      <c r="W14" s="136"/>
+      <c r="W14" s="132"/>
     </row>
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
-      <c r="C15" s="170"/>
-      <c r="D15" s="171"/>
+      <c r="C15" s="169"/>
+      <c r="D15" s="170"/>
       <c r="E15" s="35"/>
       <c r="F15" s="36"/>
       <c r="G15" s="36"/>
       <c r="H15" s="36"/>
       <c r="I15" s="83"/>
-      <c r="J15" s="149"/>
-      <c r="K15" s="150"/>
-      <c r="L15" s="151"/>
-      <c r="M15" s="151"/>
-      <c r="N15" s="151"/>
-      <c r="O15" s="151"/>
-      <c r="P15" s="151"/>
-      <c r="Q15" s="151"/>
-      <c r="R15" s="151"/>
-      <c r="S15" s="151"/>
-      <c r="T15" s="151"/>
-      <c r="U15" s="151"/>
-      <c r="V15" s="152"/>
-      <c r="W15" s="136"/>
+      <c r="J15" s="148"/>
+      <c r="K15" s="149"/>
+      <c r="L15" s="150"/>
+      <c r="M15" s="150"/>
+      <c r="N15" s="150"/>
+      <c r="O15" s="150"/>
+      <c r="P15" s="150"/>
+      <c r="Q15" s="150"/>
+      <c r="R15" s="150"/>
+      <c r="S15" s="150"/>
+      <c r="T15" s="150"/>
+      <c r="U15" s="150"/>
+      <c r="V15" s="151"/>
+      <c r="W15" s="153"/>
     </row>
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
-      <c r="C16" s="170"/>
-      <c r="D16" s="171"/>
+      <c r="C16" s="169"/>
+      <c r="D16" s="170"/>
       <c r="E16" s="30"/>
       <c r="F16" s="31"/>
       <c r="G16" s="31"/>
@@ -2602,7 +2602,7 @@
       <c r="T16" s="120"/>
       <c r="U16" s="120"/>
       <c r="V16" s="120"/>
-      <c r="W16" s="137"/>
+      <c r="W16" s="136"/>
     </row>
     <row r="17" spans="1:23" ht="12" customHeight="1">
       <c r="A17" s="32"/>
@@ -2614,26 +2614,26 @@
       <c r="G17" s="36"/>
       <c r="H17" s="36"/>
       <c r="I17" s="88"/>
-      <c r="J17" s="153"/>
-      <c r="K17" s="140"/>
-      <c r="L17" s="148"/>
-      <c r="M17" s="148"/>
-      <c r="N17" s="148"/>
-      <c r="O17" s="148"/>
-      <c r="P17" s="148"/>
-      <c r="Q17" s="148"/>
-      <c r="R17" s="148"/>
-      <c r="S17" s="148"/>
-      <c r="T17" s="148"/>
-      <c r="U17" s="148"/>
-      <c r="V17" s="148"/>
-      <c r="W17" s="154"/>
+      <c r="J17" s="152"/>
+      <c r="K17" s="139"/>
+      <c r="L17" s="147"/>
+      <c r="M17" s="147"/>
+      <c r="N17" s="147"/>
+      <c r="O17" s="147"/>
+      <c r="P17" s="147"/>
+      <c r="Q17" s="147"/>
+      <c r="R17" s="147"/>
+      <c r="S17" s="147"/>
+      <c r="T17" s="147"/>
+      <c r="U17" s="147"/>
+      <c r="V17" s="147"/>
+      <c r="W17" s="153"/>
     </row>
     <row r="18" spans="1:23" ht="12" customHeight="1">
       <c r="A18" s="18"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="170"/>
-      <c r="D18" s="171"/>
+      <c r="C18" s="169"/>
+      <c r="D18" s="170"/>
       <c r="E18" s="37"/>
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
@@ -2652,7 +2652,7 @@
       <c r="T18" s="120"/>
       <c r="U18" s="120"/>
       <c r="V18" s="120"/>
-      <c r="W18" s="137"/>
+      <c r="W18" s="136"/>
     </row>
     <row r="19" spans="1:23" ht="12" customHeight="1">
       <c r="A19" s="18"/>
@@ -2664,20 +2664,20 @@
       <c r="G19" s="40"/>
       <c r="H19" s="40"/>
       <c r="I19" s="91"/>
-      <c r="J19" s="155"/>
-      <c r="K19" s="156"/>
-      <c r="L19" s="157"/>
-      <c r="M19" s="157"/>
-      <c r="N19" s="157"/>
-      <c r="O19" s="157"/>
-      <c r="P19" s="157"/>
-      <c r="Q19" s="157"/>
-      <c r="R19" s="157"/>
-      <c r="S19" s="157"/>
-      <c r="T19" s="157"/>
-      <c r="U19" s="157"/>
-      <c r="V19" s="157"/>
-      <c r="W19" s="158"/>
+      <c r="J19" s="154"/>
+      <c r="K19" s="155"/>
+      <c r="L19" s="156"/>
+      <c r="M19" s="156"/>
+      <c r="N19" s="156"/>
+      <c r="O19" s="156"/>
+      <c r="P19" s="156"/>
+      <c r="Q19" s="156"/>
+      <c r="R19" s="156"/>
+      <c r="S19" s="156"/>
+      <c r="T19" s="156"/>
+      <c r="U19" s="156"/>
+      <c r="V19" s="156"/>
+      <c r="W19" s="157"/>
     </row>
     <row r="20" spans="1:23" ht="12" customHeight="1">
       <c r="A20" s="18"/>
@@ -2714,26 +2714,26 @@
       <c r="G21" s="48"/>
       <c r="H21" s="48"/>
       <c r="I21" s="97"/>
-      <c r="J21" s="153"/>
-      <c r="K21" s="140"/>
-      <c r="L21" s="148"/>
-      <c r="M21" s="148"/>
-      <c r="N21" s="148"/>
-      <c r="O21" s="148"/>
-      <c r="P21" s="148"/>
-      <c r="Q21" s="148"/>
-      <c r="R21" s="148"/>
-      <c r="S21" s="148"/>
-      <c r="T21" s="148"/>
-      <c r="U21" s="148"/>
-      <c r="V21" s="148"/>
-      <c r="W21" s="154"/>
+      <c r="J21" s="152"/>
+      <c r="K21" s="139"/>
+      <c r="L21" s="147"/>
+      <c r="M21" s="147"/>
+      <c r="N21" s="147"/>
+      <c r="O21" s="147"/>
+      <c r="P21" s="147"/>
+      <c r="Q21" s="147"/>
+      <c r="R21" s="147"/>
+      <c r="S21" s="147"/>
+      <c r="T21" s="147"/>
+      <c r="U21" s="147"/>
+      <c r="V21" s="147"/>
+      <c r="W21" s="153"/>
     </row>
     <row r="22" spans="1:23" ht="12" customHeight="1">
       <c r="A22" s="18"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="170"/>
-      <c r="D22" s="171"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="170"/>
       <c r="E22" s="37"/>
       <c r="F22" s="43"/>
       <c r="G22" s="43"/>
@@ -2752,7 +2752,7 @@
       <c r="T22" s="120"/>
       <c r="U22" s="120"/>
       <c r="V22" s="120"/>
-      <c r="W22" s="137"/>
+      <c r="W22" s="136"/>
     </row>
     <row r="23" spans="1:23" ht="12" customHeight="1">
       <c r="A23" s="18"/>
@@ -2764,20 +2764,20 @@
       <c r="G23" s="40"/>
       <c r="H23" s="40"/>
       <c r="I23" s="91"/>
-      <c r="J23" s="155"/>
-      <c r="K23" s="156"/>
-      <c r="L23" s="157"/>
-      <c r="M23" s="157"/>
-      <c r="N23" s="157"/>
-      <c r="O23" s="157"/>
-      <c r="P23" s="157"/>
-      <c r="Q23" s="157"/>
-      <c r="R23" s="157"/>
-      <c r="S23" s="157"/>
-      <c r="T23" s="157"/>
-      <c r="U23" s="157"/>
-      <c r="V23" s="157"/>
-      <c r="W23" s="158"/>
+      <c r="J23" s="154"/>
+      <c r="K23" s="155"/>
+      <c r="L23" s="156"/>
+      <c r="M23" s="156"/>
+      <c r="N23" s="156"/>
+      <c r="O23" s="156"/>
+      <c r="P23" s="156"/>
+      <c r="Q23" s="156"/>
+      <c r="R23" s="156"/>
+      <c r="S23" s="156"/>
+      <c r="T23" s="156"/>
+      <c r="U23" s="156"/>
+      <c r="V23" s="156"/>
+      <c r="W23" s="157"/>
     </row>
     <row r="24" spans="1:23" ht="12" customHeight="1">
       <c r="A24" s="18"/>
@@ -2814,26 +2814,26 @@
       <c r="G25" s="48"/>
       <c r="H25" s="48"/>
       <c r="I25" s="97"/>
-      <c r="J25" s="153"/>
-      <c r="K25" s="140"/>
-      <c r="L25" s="148"/>
-      <c r="M25" s="148"/>
-      <c r="N25" s="148"/>
-      <c r="O25" s="148"/>
-      <c r="P25" s="148"/>
-      <c r="Q25" s="148"/>
-      <c r="R25" s="148"/>
-      <c r="S25" s="148"/>
-      <c r="T25" s="148"/>
-      <c r="U25" s="148"/>
-      <c r="V25" s="148"/>
-      <c r="W25" s="154"/>
+      <c r="J25" s="152"/>
+      <c r="K25" s="139"/>
+      <c r="L25" s="147"/>
+      <c r="M25" s="147"/>
+      <c r="N25" s="147"/>
+      <c r="O25" s="147"/>
+      <c r="P25" s="147"/>
+      <c r="Q25" s="147"/>
+      <c r="R25" s="147"/>
+      <c r="S25" s="147"/>
+      <c r="T25" s="147"/>
+      <c r="U25" s="147"/>
+      <c r="V25" s="147"/>
+      <c r="W25" s="153"/>
     </row>
     <row r="26" spans="1:23" ht="12" customHeight="1">
       <c r="A26" s="18"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="170"/>
-      <c r="D26" s="171"/>
+      <c r="C26" s="169"/>
+      <c r="D26" s="170"/>
       <c r="E26" s="37"/>
       <c r="F26" s="43"/>
       <c r="G26" s="43"/>
@@ -2852,7 +2852,7 @@
       <c r="T26" s="120"/>
       <c r="U26" s="120"/>
       <c r="V26" s="120"/>
-      <c r="W26" s="137"/>
+      <c r="W26" s="136"/>
     </row>
     <row r="27" spans="1:23" ht="12" customHeight="1">
       <c r="A27" s="18"/>
@@ -2864,20 +2864,20 @@
       <c r="G27" s="42"/>
       <c r="H27" s="42"/>
       <c r="I27" s="92"/>
-      <c r="J27" s="155"/>
-      <c r="K27" s="156"/>
-      <c r="L27" s="157"/>
-      <c r="M27" s="157"/>
-      <c r="N27" s="157"/>
-      <c r="O27" s="157"/>
-      <c r="P27" s="157"/>
-      <c r="Q27" s="157"/>
-      <c r="R27" s="157"/>
-      <c r="S27" s="157"/>
-      <c r="T27" s="157"/>
-      <c r="U27" s="157"/>
-      <c r="V27" s="157"/>
-      <c r="W27" s="158"/>
+      <c r="J27" s="154"/>
+      <c r="K27" s="155"/>
+      <c r="L27" s="156"/>
+      <c r="M27" s="156"/>
+      <c r="N27" s="156"/>
+      <c r="O27" s="156"/>
+      <c r="P27" s="156"/>
+      <c r="Q27" s="156"/>
+      <c r="R27" s="156"/>
+      <c r="S27" s="156"/>
+      <c r="T27" s="156"/>
+      <c r="U27" s="156"/>
+      <c r="V27" s="156"/>
+      <c r="W27" s="157"/>
     </row>
     <row r="28" spans="1:23" ht="12" customHeight="1">
       <c r="A28" s="18"/>
@@ -2914,26 +2914,26 @@
       <c r="G29" s="48"/>
       <c r="H29" s="48"/>
       <c r="I29" s="97"/>
-      <c r="J29" s="153"/>
-      <c r="K29" s="140"/>
-      <c r="L29" s="148"/>
-      <c r="M29" s="148"/>
-      <c r="N29" s="148"/>
-      <c r="O29" s="148"/>
-      <c r="P29" s="148"/>
-      <c r="Q29" s="148"/>
-      <c r="R29" s="148"/>
-      <c r="S29" s="148"/>
-      <c r="T29" s="148"/>
-      <c r="U29" s="148"/>
-      <c r="V29" s="148"/>
-      <c r="W29" s="154"/>
+      <c r="J29" s="152"/>
+      <c r="K29" s="139"/>
+      <c r="L29" s="147"/>
+      <c r="M29" s="147"/>
+      <c r="N29" s="147"/>
+      <c r="O29" s="147"/>
+      <c r="P29" s="147"/>
+      <c r="Q29" s="147"/>
+      <c r="R29" s="147"/>
+      <c r="S29" s="147"/>
+      <c r="T29" s="147"/>
+      <c r="U29" s="147"/>
+      <c r="V29" s="147"/>
+      <c r="W29" s="153"/>
     </row>
     <row r="30" spans="1:23" ht="12" customHeight="1">
       <c r="A30" s="18"/>
       <c r="B30" s="18"/>
-      <c r="C30" s="170"/>
-      <c r="D30" s="171"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="170"/>
       <c r="E30" s="49"/>
       <c r="F30" s="43"/>
       <c r="G30" s="43"/>
@@ -2952,7 +2952,7 @@
       <c r="T30" s="120"/>
       <c r="U30" s="120"/>
       <c r="V30" s="120"/>
-      <c r="W30" s="137"/>
+      <c r="W30" s="136"/>
     </row>
     <row r="31" spans="1:23" ht="12" customHeight="1">
       <c r="A31" s="18"/>
@@ -2964,20 +2964,20 @@
       <c r="G31" s="42"/>
       <c r="H31" s="42"/>
       <c r="I31" s="100"/>
-      <c r="J31" s="155"/>
-      <c r="K31" s="156"/>
-      <c r="L31" s="157"/>
-      <c r="M31" s="157"/>
-      <c r="N31" s="157"/>
-      <c r="O31" s="157"/>
-      <c r="P31" s="157"/>
-      <c r="Q31" s="157"/>
-      <c r="R31" s="157"/>
-      <c r="S31" s="157"/>
-      <c r="T31" s="157"/>
-      <c r="U31" s="157"/>
-      <c r="V31" s="157"/>
-      <c r="W31" s="158"/>
+      <c r="J31" s="154"/>
+      <c r="K31" s="155"/>
+      <c r="L31" s="156"/>
+      <c r="M31" s="156"/>
+      <c r="N31" s="156"/>
+      <c r="O31" s="156"/>
+      <c r="P31" s="156"/>
+      <c r="Q31" s="156"/>
+      <c r="R31" s="156"/>
+      <c r="S31" s="156"/>
+      <c r="T31" s="156"/>
+      <c r="U31" s="156"/>
+      <c r="V31" s="156"/>
+      <c r="W31" s="157"/>
     </row>
     <row r="32" spans="1:23" ht="12" customHeight="1">
       <c r="A32" s="18"/>
@@ -3014,26 +3014,26 @@
       <c r="G33" s="48"/>
       <c r="H33" s="48"/>
       <c r="I33" s="101"/>
-      <c r="J33" s="149"/>
-      <c r="K33" s="140"/>
-      <c r="L33" s="148"/>
-      <c r="M33" s="148"/>
-      <c r="N33" s="148"/>
-      <c r="O33" s="148"/>
-      <c r="P33" s="148"/>
-      <c r="Q33" s="148"/>
-      <c r="R33" s="148"/>
-      <c r="S33" s="148"/>
-      <c r="T33" s="148"/>
-      <c r="U33" s="148"/>
-      <c r="V33" s="148"/>
-      <c r="W33" s="154"/>
+      <c r="J33" s="148"/>
+      <c r="K33" s="139"/>
+      <c r="L33" s="147"/>
+      <c r="M33" s="147"/>
+      <c r="N33" s="147"/>
+      <c r="O33" s="147"/>
+      <c r="P33" s="147"/>
+      <c r="Q33" s="147"/>
+      <c r="R33" s="147"/>
+      <c r="S33" s="147"/>
+      <c r="T33" s="147"/>
+      <c r="U33" s="147"/>
+      <c r="V33" s="147"/>
+      <c r="W33" s="153"/>
     </row>
     <row r="34" spans="1:23" ht="12" customHeight="1">
       <c r="A34" s="18"/>
       <c r="B34" s="18"/>
-      <c r="C34" s="170"/>
-      <c r="D34" s="171"/>
+      <c r="C34" s="169"/>
+      <c r="D34" s="170"/>
       <c r="E34" s="52"/>
       <c r="F34" s="53"/>
       <c r="G34" s="43"/>
@@ -3052,7 +3052,7 @@
       <c r="T34" s="103"/>
       <c r="U34" s="103"/>
       <c r="V34" s="117"/>
-      <c r="W34" s="138"/>
+      <c r="W34" s="137"/>
     </row>
     <row r="35" spans="1:23" ht="12" customHeight="1">
       <c r="A35" s="18"/>
@@ -3127,13 +3127,13 @@
       <c r="T37" s="107"/>
       <c r="U37" s="107"/>
       <c r="V37" s="96"/>
-      <c r="W37" s="139"/>
+      <c r="W37" s="138"/>
     </row>
     <row r="38" spans="1:23" ht="12" customHeight="1">
       <c r="A38" s="18"/>
       <c r="B38" s="18"/>
-      <c r="C38" s="170"/>
-      <c r="D38" s="171"/>
+      <c r="C38" s="169"/>
+      <c r="D38" s="170"/>
       <c r="E38" s="54"/>
       <c r="F38" s="55"/>
       <c r="G38" s="55"/>
@@ -3152,7 +3152,7 @@
       <c r="T38" s="120"/>
       <c r="U38" s="120"/>
       <c r="V38" s="120"/>
-      <c r="W38" s="137"/>
+      <c r="W38" s="136"/>
     </row>
     <row r="39" spans="1:23" ht="12" customHeight="1">
       <c r="A39" s="18"/>
@@ -3164,20 +3164,20 @@
       <c r="G39" s="17"/>
       <c r="H39" s="17"/>
       <c r="I39" s="100"/>
-      <c r="J39" s="155"/>
-      <c r="K39" s="156"/>
-      <c r="L39" s="157"/>
-      <c r="M39" s="157"/>
-      <c r="N39" s="157"/>
-      <c r="O39" s="157"/>
-      <c r="P39" s="157"/>
-      <c r="Q39" s="157"/>
-      <c r="R39" s="157"/>
-      <c r="S39" s="157"/>
-      <c r="T39" s="157"/>
-      <c r="U39" s="157"/>
-      <c r="V39" s="157"/>
-      <c r="W39" s="158"/>
+      <c r="J39" s="154"/>
+      <c r="K39" s="155"/>
+      <c r="L39" s="156"/>
+      <c r="M39" s="156"/>
+      <c r="N39" s="156"/>
+      <c r="O39" s="156"/>
+      <c r="P39" s="156"/>
+      <c r="Q39" s="156"/>
+      <c r="R39" s="156"/>
+      <c r="S39" s="156"/>
+      <c r="T39" s="156"/>
+      <c r="U39" s="156"/>
+      <c r="V39" s="156"/>
+      <c r="W39" s="157"/>
     </row>
     <row r="40" spans="1:23" ht="12" customHeight="1">
       <c r="A40" s="18"/>
@@ -3214,26 +3214,26 @@
       <c r="G41" s="48"/>
       <c r="H41" s="58"/>
       <c r="I41" s="101"/>
-      <c r="J41" s="153"/>
-      <c r="K41" s="140"/>
-      <c r="L41" s="148"/>
-      <c r="M41" s="148"/>
-      <c r="N41" s="148"/>
-      <c r="O41" s="148"/>
-      <c r="P41" s="148"/>
-      <c r="Q41" s="148"/>
-      <c r="R41" s="148"/>
-      <c r="S41" s="148"/>
-      <c r="T41" s="148"/>
-      <c r="U41" s="148"/>
-      <c r="V41" s="148"/>
-      <c r="W41" s="154"/>
+      <c r="J41" s="152"/>
+      <c r="K41" s="139"/>
+      <c r="L41" s="147"/>
+      <c r="M41" s="147"/>
+      <c r="N41" s="147"/>
+      <c r="O41" s="147"/>
+      <c r="P41" s="147"/>
+      <c r="Q41" s="147"/>
+      <c r="R41" s="147"/>
+      <c r="S41" s="147"/>
+      <c r="T41" s="147"/>
+      <c r="U41" s="147"/>
+      <c r="V41" s="147"/>
+      <c r="W41" s="153"/>
     </row>
     <row r="42" spans="1:23" ht="12" customHeight="1">
       <c r="A42" s="18"/>
       <c r="B42" s="18"/>
-      <c r="C42" s="170"/>
-      <c r="D42" s="171"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="170"/>
       <c r="E42" s="54"/>
       <c r="F42" s="55"/>
       <c r="G42" s="55"/>
@@ -3252,7 +3252,7 @@
       <c r="T42" s="120"/>
       <c r="U42" s="120"/>
       <c r="V42" s="120"/>
-      <c r="W42" s="137"/>
+      <c r="W42" s="136"/>
     </row>
     <row r="43" spans="1:23" ht="12" customHeight="1">
       <c r="A43" s="18"/>
@@ -3264,20 +3264,20 @@
       <c r="G43" s="17"/>
       <c r="H43" s="17"/>
       <c r="I43" s="100"/>
-      <c r="J43" s="155"/>
-      <c r="K43" s="156"/>
-      <c r="L43" s="157"/>
-      <c r="M43" s="157"/>
-      <c r="N43" s="157"/>
-      <c r="O43" s="157"/>
-      <c r="P43" s="157"/>
-      <c r="Q43" s="157"/>
-      <c r="R43" s="157"/>
-      <c r="S43" s="157"/>
-      <c r="T43" s="157"/>
-      <c r="U43" s="157"/>
-      <c r="V43" s="157"/>
-      <c r="W43" s="158"/>
+      <c r="J43" s="154"/>
+      <c r="K43" s="155"/>
+      <c r="L43" s="156"/>
+      <c r="M43" s="156"/>
+      <c r="N43" s="156"/>
+      <c r="O43" s="156"/>
+      <c r="P43" s="156"/>
+      <c r="Q43" s="156"/>
+      <c r="R43" s="156"/>
+      <c r="S43" s="156"/>
+      <c r="T43" s="156"/>
+      <c r="U43" s="156"/>
+      <c r="V43" s="156"/>
+      <c r="W43" s="157"/>
     </row>
     <row r="44" spans="1:23" ht="12" customHeight="1">
       <c r="A44" s="18"/>
@@ -3314,26 +3314,26 @@
       <c r="G45" s="48"/>
       <c r="H45" s="48"/>
       <c r="I45" s="101"/>
-      <c r="J45" s="153"/>
-      <c r="K45" s="140"/>
-      <c r="L45" s="148"/>
-      <c r="M45" s="148"/>
-      <c r="N45" s="148"/>
-      <c r="O45" s="148"/>
-      <c r="P45" s="148"/>
-      <c r="Q45" s="148"/>
-      <c r="R45" s="148"/>
-      <c r="S45" s="148"/>
-      <c r="T45" s="148"/>
-      <c r="U45" s="148"/>
-      <c r="V45" s="148"/>
-      <c r="W45" s="154"/>
+      <c r="J45" s="152"/>
+      <c r="K45" s="139"/>
+      <c r="L45" s="147"/>
+      <c r="M45" s="147"/>
+      <c r="N45" s="147"/>
+      <c r="O45" s="147"/>
+      <c r="P45" s="147"/>
+      <c r="Q45" s="147"/>
+      <c r="R45" s="147"/>
+      <c r="S45" s="147"/>
+      <c r="T45" s="147"/>
+      <c r="U45" s="147"/>
+      <c r="V45" s="147"/>
+      <c r="W45" s="153"/>
     </row>
     <row r="46" spans="1:23" ht="12" customHeight="1">
       <c r="A46" s="18"/>
       <c r="B46" s="18"/>
-      <c r="C46" s="170"/>
-      <c r="D46" s="171"/>
+      <c r="C46" s="169"/>
+      <c r="D46" s="170"/>
       <c r="E46" s="37"/>
       <c r="F46" s="59"/>
       <c r="G46" s="55"/>
@@ -3352,7 +3352,7 @@
       <c r="T46" s="120"/>
       <c r="U46" s="120"/>
       <c r="V46" s="120"/>
-      <c r="W46" s="137"/>
+      <c r="W46" s="136"/>
     </row>
     <row r="47" spans="1:23" ht="12" customHeight="1">
       <c r="A47" s="18"/>
@@ -3364,20 +3364,20 @@
       <c r="G47" s="17"/>
       <c r="H47" s="17"/>
       <c r="I47" s="112"/>
-      <c r="J47" s="155"/>
-      <c r="K47" s="156"/>
-      <c r="L47" s="157"/>
-      <c r="M47" s="157"/>
-      <c r="N47" s="157"/>
-      <c r="O47" s="157"/>
-      <c r="P47" s="157"/>
-      <c r="Q47" s="157"/>
-      <c r="R47" s="157"/>
-      <c r="S47" s="157"/>
-      <c r="T47" s="157"/>
-      <c r="U47" s="157"/>
-      <c r="V47" s="157"/>
-      <c r="W47" s="158"/>
+      <c r="J47" s="154"/>
+      <c r="K47" s="155"/>
+      <c r="L47" s="156"/>
+      <c r="M47" s="156"/>
+      <c r="N47" s="156"/>
+      <c r="O47" s="156"/>
+      <c r="P47" s="156"/>
+      <c r="Q47" s="156"/>
+      <c r="R47" s="156"/>
+      <c r="S47" s="156"/>
+      <c r="T47" s="156"/>
+      <c r="U47" s="156"/>
+      <c r="V47" s="156"/>
+      <c r="W47" s="157"/>
     </row>
     <row r="48" spans="1:23" ht="12" customHeight="1">
       <c r="A48" s="18"/>
@@ -3414,26 +3414,26 @@
       <c r="G49" s="47"/>
       <c r="H49" s="58"/>
       <c r="I49" s="101"/>
-      <c r="J49" s="153"/>
-      <c r="K49" s="140"/>
-      <c r="L49" s="148"/>
-      <c r="M49" s="148"/>
-      <c r="N49" s="148"/>
-      <c r="O49" s="148"/>
-      <c r="P49" s="148"/>
-      <c r="Q49" s="148"/>
-      <c r="R49" s="148"/>
-      <c r="S49" s="148"/>
-      <c r="T49" s="148"/>
-      <c r="U49" s="148"/>
-      <c r="V49" s="148"/>
-      <c r="W49" s="154"/>
+      <c r="J49" s="152"/>
+      <c r="K49" s="139"/>
+      <c r="L49" s="147"/>
+      <c r="M49" s="147"/>
+      <c r="N49" s="147"/>
+      <c r="O49" s="147"/>
+      <c r="P49" s="147"/>
+      <c r="Q49" s="147"/>
+      <c r="R49" s="147"/>
+      <c r="S49" s="147"/>
+      <c r="T49" s="147"/>
+      <c r="U49" s="147"/>
+      <c r="V49" s="147"/>
+      <c r="W49" s="153"/>
     </row>
     <row r="50" spans="1:23" ht="12" customHeight="1">
       <c r="A50" s="18"/>
       <c r="B50" s="18"/>
-      <c r="C50" s="170"/>
-      <c r="D50" s="171"/>
+      <c r="C50" s="169"/>
+      <c r="D50" s="170"/>
       <c r="E50" s="37"/>
       <c r="F50" s="59"/>
       <c r="G50" s="55"/>
@@ -3452,7 +3452,7 @@
       <c r="T50" s="120"/>
       <c r="U50" s="120"/>
       <c r="V50" s="120"/>
-      <c r="W50" s="137"/>
+      <c r="W50" s="136"/>
     </row>
     <row r="51" spans="1:23" ht="12" customHeight="1">
       <c r="A51" s="18"/>
@@ -3464,20 +3464,20 @@
       <c r="G51" s="17"/>
       <c r="H51" s="17"/>
       <c r="I51" s="112"/>
-      <c r="J51" s="155"/>
-      <c r="K51" s="156"/>
-      <c r="L51" s="157"/>
-      <c r="M51" s="157"/>
-      <c r="N51" s="157"/>
-      <c r="O51" s="157"/>
-      <c r="P51" s="157"/>
-      <c r="Q51" s="157"/>
-      <c r="R51" s="157"/>
-      <c r="S51" s="157"/>
-      <c r="T51" s="157"/>
-      <c r="U51" s="157"/>
-      <c r="V51" s="157"/>
-      <c r="W51" s="158"/>
+      <c r="J51" s="154"/>
+      <c r="K51" s="155"/>
+      <c r="L51" s="156"/>
+      <c r="M51" s="156"/>
+      <c r="N51" s="156"/>
+      <c r="O51" s="156"/>
+      <c r="P51" s="156"/>
+      <c r="Q51" s="156"/>
+      <c r="R51" s="156"/>
+      <c r="S51" s="156"/>
+      <c r="T51" s="156"/>
+      <c r="U51" s="156"/>
+      <c r="V51" s="156"/>
+      <c r="W51" s="157"/>
     </row>
     <row r="52" spans="1:23" ht="12" customHeight="1">
       <c r="A52" s="18"/>
@@ -3514,20 +3514,20 @@
       <c r="G53" s="47"/>
       <c r="H53" s="58"/>
       <c r="I53" s="101"/>
-      <c r="J53" s="149"/>
-      <c r="K53" s="159"/>
-      <c r="L53" s="160"/>
-      <c r="M53" s="160"/>
-      <c r="N53" s="160"/>
-      <c r="O53" s="160"/>
-      <c r="P53" s="160"/>
-      <c r="Q53" s="160"/>
-      <c r="R53" s="160"/>
-      <c r="S53" s="160"/>
-      <c r="T53" s="160"/>
-      <c r="U53" s="160"/>
-      <c r="V53" s="160"/>
-      <c r="W53" s="161"/>
+      <c r="J53" s="148"/>
+      <c r="K53" s="158"/>
+      <c r="L53" s="159"/>
+      <c r="M53" s="159"/>
+      <c r="N53" s="159"/>
+      <c r="O53" s="159"/>
+      <c r="P53" s="159"/>
+      <c r="Q53" s="159"/>
+      <c r="R53" s="159"/>
+      <c r="S53" s="159"/>
+      <c r="T53" s="159"/>
+      <c r="U53" s="159"/>
+      <c r="V53" s="159"/>
+      <c r="W53" s="160"/>
     </row>
     <row r="54" spans="1:23" ht="12" customHeight="1">
       <c r="C54" s="125"/>
@@ -3668,27 +3668,27 @@
       <c r="W59" s="129"/>
     </row>
     <row r="64" spans="1:23" ht="12" customHeight="1">
-      <c r="C64" s="170"/>
-      <c r="D64" s="171"/>
+      <c r="C64" s="169"/>
+      <c r="D64" s="170"/>
       <c r="E64" s="30"/>
       <c r="F64" s="31"/>
       <c r="G64" s="31"/>
       <c r="H64" s="31"/>
       <c r="I64" s="87"/>
-      <c r="J64" s="167"/>
-      <c r="K64" s="165"/>
-      <c r="L64" s="141"/>
-      <c r="M64" s="141"/>
-      <c r="N64" s="141"/>
-      <c r="O64" s="141"/>
-      <c r="P64" s="141"/>
-      <c r="Q64" s="141"/>
-      <c r="R64" s="141"/>
-      <c r="S64" s="141"/>
-      <c r="T64" s="141"/>
-      <c r="U64" s="141"/>
-      <c r="V64" s="141"/>
-      <c r="W64" s="166"/>
+      <c r="J64" s="166"/>
+      <c r="K64" s="164"/>
+      <c r="L64" s="140"/>
+      <c r="M64" s="140"/>
+      <c r="N64" s="140"/>
+      <c r="O64" s="140"/>
+      <c r="P64" s="140"/>
+      <c r="Q64" s="140"/>
+      <c r="R64" s="140"/>
+      <c r="S64" s="140"/>
+      <c r="T64" s="140"/>
+      <c r="U64" s="140"/>
+      <c r="V64" s="140"/>
+      <c r="W64" s="165"/>
     </row>
     <row r="65" spans="1:23" ht="12" customHeight="1">
       <c r="C65" s="33"/>
@@ -3711,32 +3711,32 @@
       <c r="T65" s="90"/>
       <c r="U65" s="90"/>
       <c r="V65" s="90"/>
-      <c r="W65" s="139"/>
+      <c r="W65" s="132"/>
     </row>
     <row r="66" spans="1:23" ht="12" customHeight="1">
       <c r="A66" s="122"/>
       <c r="B66" s="122"/>
-      <c r="C66" s="170"/>
-      <c r="D66" s="171"/>
+      <c r="C66" s="169"/>
+      <c r="D66" s="170"/>
       <c r="E66" s="37"/>
       <c r="F66" s="43"/>
       <c r="G66" s="43"/>
       <c r="H66" s="43"/>
       <c r="I66" s="93"/>
-      <c r="J66" s="167"/>
-      <c r="K66" s="165"/>
-      <c r="L66" s="141"/>
-      <c r="M66" s="141"/>
-      <c r="N66" s="141"/>
-      <c r="O66" s="141"/>
-      <c r="P66" s="141"/>
-      <c r="Q66" s="141"/>
-      <c r="R66" s="141"/>
-      <c r="S66" s="141"/>
-      <c r="T66" s="141"/>
-      <c r="U66" s="141"/>
-      <c r="V66" s="141"/>
-      <c r="W66" s="166"/>
+      <c r="J66" s="166"/>
+      <c r="K66" s="164"/>
+      <c r="L66" s="140"/>
+      <c r="M66" s="140"/>
+      <c r="N66" s="140"/>
+      <c r="O66" s="140"/>
+      <c r="P66" s="140"/>
+      <c r="Q66" s="140"/>
+      <c r="R66" s="140"/>
+      <c r="S66" s="140"/>
+      <c r="T66" s="140"/>
+      <c r="U66" s="140"/>
+      <c r="V66" s="140"/>
+      <c r="W66" s="165"/>
     </row>
     <row r="67" spans="1:23" ht="12" customHeight="1">
       <c r="A67" s="122"/>
@@ -3773,20 +3773,20 @@
       <c r="G68" s="42"/>
       <c r="H68" s="42"/>
       <c r="I68" s="92"/>
-      <c r="J68" s="153"/>
-      <c r="K68" s="140"/>
-      <c r="L68" s="148"/>
-      <c r="M68" s="148"/>
-      <c r="N68" s="148"/>
-      <c r="O68" s="148"/>
-      <c r="P68" s="148"/>
-      <c r="Q68" s="148"/>
-      <c r="R68" s="148"/>
-      <c r="S68" s="148"/>
-      <c r="T68" s="148"/>
-      <c r="U68" s="148"/>
-      <c r="V68" s="169"/>
-      <c r="W68" s="133"/>
+      <c r="J68" s="152"/>
+      <c r="K68" s="139"/>
+      <c r="L68" s="147"/>
+      <c r="M68" s="147"/>
+      <c r="N68" s="147"/>
+      <c r="O68" s="147"/>
+      <c r="P68" s="147"/>
+      <c r="Q68" s="147"/>
+      <c r="R68" s="147"/>
+      <c r="S68" s="147"/>
+      <c r="T68" s="147"/>
+      <c r="U68" s="147"/>
+      <c r="V68" s="168"/>
+      <c r="W68" s="153"/>
     </row>
     <row r="69" spans="1:23" ht="12" customHeight="1">
       <c r="A69" s="122"/>
@@ -3811,32 +3811,32 @@
       <c r="T69" s="90"/>
       <c r="U69" s="90"/>
       <c r="V69" s="90"/>
-      <c r="W69" s="139"/>
+      <c r="W69" s="132"/>
     </row>
     <row r="70" spans="1:23" ht="12" customHeight="1">
       <c r="A70" s="122"/>
       <c r="B70" s="122"/>
-      <c r="C70" s="170"/>
-      <c r="D70" s="171"/>
+      <c r="C70" s="169"/>
+      <c r="D70" s="170"/>
       <c r="E70" s="37"/>
       <c r="F70" s="43"/>
       <c r="G70" s="43"/>
       <c r="H70" s="43"/>
       <c r="I70" s="98"/>
-      <c r="J70" s="167"/>
-      <c r="K70" s="165"/>
-      <c r="L70" s="141"/>
-      <c r="M70" s="141"/>
-      <c r="N70" s="141"/>
-      <c r="O70" s="141"/>
-      <c r="P70" s="141"/>
-      <c r="Q70" s="141"/>
-      <c r="R70" s="141"/>
-      <c r="S70" s="141"/>
-      <c r="T70" s="141"/>
-      <c r="U70" s="141"/>
-      <c r="V70" s="168"/>
-      <c r="W70" s="138"/>
+      <c r="J70" s="166"/>
+      <c r="K70" s="164"/>
+      <c r="L70" s="140"/>
+      <c r="M70" s="140"/>
+      <c r="N70" s="140"/>
+      <c r="O70" s="140"/>
+      <c r="P70" s="140"/>
+      <c r="Q70" s="140"/>
+      <c r="R70" s="140"/>
+      <c r="S70" s="140"/>
+      <c r="T70" s="140"/>
+      <c r="U70" s="140"/>
+      <c r="V70" s="167"/>
+      <c r="W70" s="165"/>
     </row>
     <row r="71" spans="1:23" ht="12" customHeight="1">
       <c r="A71" s="122"/>
@@ -3873,20 +3873,20 @@
       <c r="G72" s="42"/>
       <c r="H72" s="42"/>
       <c r="I72" s="92"/>
-      <c r="J72" s="153"/>
-      <c r="K72" s="140"/>
-      <c r="L72" s="148"/>
-      <c r="M72" s="148"/>
-      <c r="N72" s="148"/>
-      <c r="O72" s="148"/>
-      <c r="P72" s="148"/>
-      <c r="Q72" s="148"/>
-      <c r="R72" s="148"/>
-      <c r="S72" s="148"/>
-      <c r="T72" s="148"/>
-      <c r="U72" s="148"/>
-      <c r="V72" s="148"/>
-      <c r="W72" s="128"/>
+      <c r="J72" s="152"/>
+      <c r="K72" s="139"/>
+      <c r="L72" s="147"/>
+      <c r="M72" s="147"/>
+      <c r="N72" s="147"/>
+      <c r="O72" s="147"/>
+      <c r="P72" s="147"/>
+      <c r="Q72" s="147"/>
+      <c r="R72" s="147"/>
+      <c r="S72" s="147"/>
+      <c r="T72" s="147"/>
+      <c r="U72" s="147"/>
+      <c r="V72" s="147"/>
+      <c r="W72" s="153"/>
     </row>
     <row r="73" spans="1:23" ht="12" customHeight="1">
       <c r="A73" s="122"/>
@@ -3911,32 +3911,32 @@
       <c r="T73" s="90"/>
       <c r="U73" s="90"/>
       <c r="V73" s="90"/>
-      <c r="W73" s="139"/>
+      <c r="W73" s="132"/>
     </row>
     <row r="74" spans="1:23" ht="12" customHeight="1">
       <c r="A74" s="122"/>
       <c r="B74" s="122"/>
-      <c r="C74" s="170"/>
-      <c r="D74" s="171"/>
+      <c r="C74" s="169"/>
+      <c r="D74" s="170"/>
       <c r="E74" s="49"/>
       <c r="F74" s="43"/>
       <c r="G74" s="43"/>
       <c r="H74" s="43"/>
       <c r="I74" s="99"/>
-      <c r="J74" s="167"/>
-      <c r="K74" s="165"/>
-      <c r="L74" s="141"/>
-      <c r="M74" s="141"/>
-      <c r="N74" s="141"/>
-      <c r="O74" s="141"/>
-      <c r="P74" s="141"/>
-      <c r="Q74" s="141"/>
-      <c r="R74" s="141"/>
-      <c r="S74" s="141"/>
-      <c r="T74" s="141"/>
-      <c r="U74" s="141"/>
-      <c r="V74" s="141"/>
-      <c r="W74" s="138"/>
+      <c r="J74" s="166"/>
+      <c r="K74" s="164"/>
+      <c r="L74" s="140"/>
+      <c r="M74" s="140"/>
+      <c r="N74" s="140"/>
+      <c r="O74" s="140"/>
+      <c r="P74" s="140"/>
+      <c r="Q74" s="140"/>
+      <c r="R74" s="140"/>
+      <c r="S74" s="140"/>
+      <c r="T74" s="140"/>
+      <c r="U74" s="140"/>
+      <c r="V74" s="140"/>
+      <c r="W74" s="165"/>
     </row>
     <row r="75" spans="1:23" ht="12" customHeight="1">
       <c r="A75" s="122"/>
@@ -3961,7 +3961,7 @@
       <c r="T75" s="72"/>
       <c r="U75" s="72"/>
       <c r="V75" s="72"/>
-      <c r="W75" s="134"/>
+      <c r="W75" s="132"/>
     </row>
     <row r="76" spans="1:23" ht="12" customHeight="1">
       <c r="A76" s="122"/>
@@ -3973,20 +3973,20 @@
       <c r="G76" s="42"/>
       <c r="H76" s="42"/>
       <c r="I76" s="100"/>
-      <c r="J76" s="153"/>
-      <c r="K76" s="140"/>
-      <c r="L76" s="148"/>
-      <c r="M76" s="148"/>
-      <c r="N76" s="148"/>
-      <c r="O76" s="148"/>
-      <c r="P76" s="148"/>
-      <c r="Q76" s="148"/>
-      <c r="R76" s="148"/>
-      <c r="S76" s="148"/>
-      <c r="T76" s="148"/>
-      <c r="U76" s="148"/>
-      <c r="V76" s="148"/>
-      <c r="W76" s="154"/>
+      <c r="J76" s="152"/>
+      <c r="K76" s="139"/>
+      <c r="L76" s="147"/>
+      <c r="M76" s="147"/>
+      <c r="N76" s="147"/>
+      <c r="O76" s="147"/>
+      <c r="P76" s="147"/>
+      <c r="Q76" s="147"/>
+      <c r="R76" s="147"/>
+      <c r="S76" s="147"/>
+      <c r="T76" s="147"/>
+      <c r="U76" s="147"/>
+      <c r="V76" s="147"/>
+      <c r="W76" s="153"/>
     </row>
     <row r="77" spans="1:23" ht="12" customHeight="1">
       <c r="A77" s="122"/>
@@ -4011,19 +4011,19 @@
       <c r="T77" s="90"/>
       <c r="U77" s="90"/>
       <c r="V77" s="90"/>
-      <c r="W77" s="139"/>
+      <c r="W77" s="132"/>
     </row>
     <row r="78" spans="1:23" ht="12" customHeight="1">
       <c r="A78" s="122"/>
       <c r="B78" s="122"/>
-      <c r="C78" s="170"/>
-      <c r="D78" s="171"/>
+      <c r="C78" s="169"/>
+      <c r="D78" s="170"/>
       <c r="E78" s="52"/>
       <c r="F78" s="53"/>
       <c r="G78" s="43"/>
       <c r="H78" s="53"/>
       <c r="I78" s="99"/>
-      <c r="J78" s="167"/>
+      <c r="J78" s="166"/>
       <c r="K78" s="102"/>
       <c r="L78" s="103"/>
       <c r="M78" s="103"/>
@@ -4035,8 +4035,8 @@
       <c r="S78" s="103"/>
       <c r="T78" s="103"/>
       <c r="U78" s="103"/>
-      <c r="V78" s="141"/>
-      <c r="W78" s="138"/>
+      <c r="V78" s="140"/>
+      <c r="W78" s="137"/>
     </row>
     <row r="79" spans="1:23" ht="12" customHeight="1">
       <c r="A79" s="122"/>
@@ -4073,20 +4073,20 @@
       <c r="G80" s="42"/>
       <c r="H80" s="42"/>
       <c r="I80" s="100"/>
-      <c r="J80" s="153"/>
-      <c r="K80" s="140"/>
-      <c r="L80" s="148"/>
-      <c r="M80" s="148"/>
-      <c r="N80" s="148"/>
-      <c r="O80" s="148"/>
-      <c r="P80" s="148"/>
-      <c r="Q80" s="148"/>
-      <c r="R80" s="148"/>
-      <c r="S80" s="148"/>
-      <c r="T80" s="148"/>
-      <c r="U80" s="148"/>
-      <c r="V80" s="148"/>
-      <c r="W80" s="154"/>
+      <c r="J80" s="152"/>
+      <c r="K80" s="139"/>
+      <c r="L80" s="147"/>
+      <c r="M80" s="147"/>
+      <c r="N80" s="147"/>
+      <c r="O80" s="147"/>
+      <c r="P80" s="147"/>
+      <c r="Q80" s="147"/>
+      <c r="R80" s="147"/>
+      <c r="S80" s="147"/>
+      <c r="T80" s="147"/>
+      <c r="U80" s="147"/>
+      <c r="V80" s="147"/>
+      <c r="W80" s="153"/>
     </row>
     <row r="81" spans="1:23" ht="12" customHeight="1">
       <c r="A81" s="122"/>
@@ -4111,32 +4111,32 @@
       <c r="T81" s="107"/>
       <c r="U81" s="107"/>
       <c r="V81" s="90"/>
-      <c r="W81" s="139"/>
+      <c r="W81" s="138"/>
     </row>
     <row r="82" spans="1:23" ht="12" customHeight="1">
       <c r="A82" s="122"/>
       <c r="B82" s="122"/>
-      <c r="C82" s="170"/>
-      <c r="D82" s="171"/>
+      <c r="C82" s="169"/>
+      <c r="D82" s="170"/>
       <c r="E82" s="54"/>
       <c r="F82" s="55"/>
       <c r="G82" s="55"/>
       <c r="H82" s="55"/>
       <c r="I82" s="99"/>
-      <c r="J82" s="164"/>
-      <c r="K82" s="165"/>
-      <c r="L82" s="141"/>
-      <c r="M82" s="141"/>
-      <c r="N82" s="141"/>
-      <c r="O82" s="141"/>
-      <c r="P82" s="141"/>
-      <c r="Q82" s="141"/>
-      <c r="R82" s="141"/>
-      <c r="S82" s="141"/>
-      <c r="T82" s="141"/>
-      <c r="U82" s="141"/>
-      <c r="V82" s="141"/>
-      <c r="W82" s="166"/>
+      <c r="J82" s="163"/>
+      <c r="K82" s="164"/>
+      <c r="L82" s="140"/>
+      <c r="M82" s="140"/>
+      <c r="N82" s="140"/>
+      <c r="O82" s="140"/>
+      <c r="P82" s="140"/>
+      <c r="Q82" s="140"/>
+      <c r="R82" s="140"/>
+      <c r="S82" s="140"/>
+      <c r="T82" s="140"/>
+      <c r="U82" s="140"/>
+      <c r="V82" s="140"/>
+      <c r="W82" s="165"/>
     </row>
     <row r="83" spans="1:23" ht="12" customHeight="1">
       <c r="A83" s="122"/>
@@ -4173,20 +4173,20 @@
       <c r="G84" s="42"/>
       <c r="H84" s="57"/>
       <c r="I84" s="100"/>
-      <c r="J84" s="162"/>
-      <c r="K84" s="140"/>
-      <c r="L84" s="148"/>
-      <c r="M84" s="148"/>
-      <c r="N84" s="148"/>
-      <c r="O84" s="148"/>
-      <c r="P84" s="148"/>
-      <c r="Q84" s="148"/>
-      <c r="R84" s="148"/>
-      <c r="S84" s="148"/>
-      <c r="T84" s="148"/>
-      <c r="U84" s="148"/>
-      <c r="V84" s="148"/>
-      <c r="W84" s="128"/>
+      <c r="J84" s="161"/>
+      <c r="K84" s="139"/>
+      <c r="L84" s="147"/>
+      <c r="M84" s="147"/>
+      <c r="N84" s="147"/>
+      <c r="O84" s="147"/>
+      <c r="P84" s="147"/>
+      <c r="Q84" s="147"/>
+      <c r="R84" s="147"/>
+      <c r="S84" s="147"/>
+      <c r="T84" s="147"/>
+      <c r="U84" s="147"/>
+      <c r="V84" s="147"/>
+      <c r="W84" s="153"/>
     </row>
     <row r="85" spans="1:23" ht="12" customHeight="1">
       <c r="A85" s="122"/>
@@ -4211,32 +4211,32 @@
       <c r="T85" s="90"/>
       <c r="U85" s="90"/>
       <c r="V85" s="90"/>
-      <c r="W85" s="139"/>
+      <c r="W85" s="132"/>
     </row>
     <row r="86" spans="1:23" ht="12" customHeight="1">
       <c r="A86" s="122"/>
       <c r="B86" s="122"/>
-      <c r="C86" s="170"/>
-      <c r="D86" s="171"/>
+      <c r="C86" s="169"/>
+      <c r="D86" s="170"/>
       <c r="E86" s="54"/>
       <c r="F86" s="55"/>
       <c r="G86" s="55"/>
       <c r="H86" s="55"/>
       <c r="I86" s="99"/>
-      <c r="J86" s="164"/>
-      <c r="K86" s="165"/>
-      <c r="L86" s="141"/>
-      <c r="M86" s="141"/>
-      <c r="N86" s="141"/>
-      <c r="O86" s="141"/>
-      <c r="P86" s="141"/>
-      <c r="Q86" s="141"/>
-      <c r="R86" s="141"/>
-      <c r="S86" s="141"/>
-      <c r="T86" s="141"/>
-      <c r="U86" s="141"/>
-      <c r="V86" s="141"/>
-      <c r="W86" s="166"/>
+      <c r="J86" s="163"/>
+      <c r="K86" s="164"/>
+      <c r="L86" s="140"/>
+      <c r="M86" s="140"/>
+      <c r="N86" s="140"/>
+      <c r="O86" s="140"/>
+      <c r="P86" s="140"/>
+      <c r="Q86" s="140"/>
+      <c r="R86" s="140"/>
+      <c r="S86" s="140"/>
+      <c r="T86" s="140"/>
+      <c r="U86" s="140"/>
+      <c r="V86" s="140"/>
+      <c r="W86" s="165"/>
     </row>
     <row r="87" spans="1:23" ht="12" customHeight="1">
       <c r="A87" s="122"/>
@@ -4273,20 +4273,20 @@
       <c r="G88" s="42"/>
       <c r="H88" s="57"/>
       <c r="I88" s="100"/>
-      <c r="J88" s="162"/>
-      <c r="K88" s="140"/>
-      <c r="L88" s="148"/>
-      <c r="M88" s="148"/>
-      <c r="N88" s="148"/>
-      <c r="O88" s="148"/>
-      <c r="P88" s="148"/>
-      <c r="Q88" s="148"/>
-      <c r="R88" s="148"/>
-      <c r="S88" s="148"/>
-      <c r="T88" s="148"/>
-      <c r="U88" s="148"/>
-      <c r="V88" s="148"/>
-      <c r="W88" s="128"/>
+      <c r="J88" s="161"/>
+      <c r="K88" s="139"/>
+      <c r="L88" s="147"/>
+      <c r="M88" s="147"/>
+      <c r="N88" s="147"/>
+      <c r="O88" s="147"/>
+      <c r="P88" s="147"/>
+      <c r="Q88" s="147"/>
+      <c r="R88" s="147"/>
+      <c r="S88" s="147"/>
+      <c r="T88" s="147"/>
+      <c r="U88" s="147"/>
+      <c r="V88" s="147"/>
+      <c r="W88" s="153"/>
     </row>
     <row r="89" spans="1:23" ht="12" customHeight="1">
       <c r="A89" s="122"/>
@@ -4311,32 +4311,32 @@
       <c r="T89" s="90"/>
       <c r="U89" s="90"/>
       <c r="V89" s="90"/>
-      <c r="W89" s="139"/>
+      <c r="W89" s="132"/>
     </row>
     <row r="90" spans="1:23" ht="12" customHeight="1">
       <c r="A90" s="122"/>
       <c r="B90" s="122"/>
-      <c r="C90" s="170"/>
-      <c r="D90" s="171"/>
+      <c r="C90" s="169"/>
+      <c r="D90" s="170"/>
       <c r="E90" s="37"/>
       <c r="F90" s="59"/>
       <c r="G90" s="55"/>
       <c r="H90" s="55"/>
       <c r="I90" s="111"/>
-      <c r="J90" s="164"/>
-      <c r="K90" s="165"/>
-      <c r="L90" s="141"/>
-      <c r="M90" s="141"/>
-      <c r="N90" s="141"/>
-      <c r="O90" s="141"/>
-      <c r="P90" s="141"/>
-      <c r="Q90" s="141"/>
-      <c r="R90" s="141"/>
-      <c r="S90" s="141"/>
-      <c r="T90" s="141"/>
-      <c r="U90" s="141"/>
-      <c r="V90" s="141"/>
-      <c r="W90" s="166"/>
+      <c r="J90" s="163"/>
+      <c r="K90" s="164"/>
+      <c r="L90" s="140"/>
+      <c r="M90" s="140"/>
+      <c r="N90" s="140"/>
+      <c r="O90" s="140"/>
+      <c r="P90" s="140"/>
+      <c r="Q90" s="140"/>
+      <c r="R90" s="140"/>
+      <c r="S90" s="140"/>
+      <c r="T90" s="140"/>
+      <c r="U90" s="140"/>
+      <c r="V90" s="140"/>
+      <c r="W90" s="165"/>
     </row>
     <row r="91" spans="1:23" ht="12" customHeight="1">
       <c r="A91" s="122"/>
@@ -4373,20 +4373,20 @@
       <c r="G92" s="61"/>
       <c r="H92" s="62"/>
       <c r="I92" s="100"/>
-      <c r="J92" s="162"/>
-      <c r="K92" s="163"/>
-      <c r="L92" s="148"/>
-      <c r="M92" s="148"/>
-      <c r="N92" s="148"/>
-      <c r="O92" s="148"/>
-      <c r="P92" s="148"/>
-      <c r="Q92" s="148"/>
-      <c r="R92" s="148"/>
-      <c r="S92" s="148"/>
-      <c r="T92" s="148"/>
-      <c r="U92" s="148"/>
-      <c r="V92" s="148"/>
-      <c r="W92" s="133"/>
+      <c r="J92" s="161"/>
+      <c r="K92" s="162"/>
+      <c r="L92" s="147"/>
+      <c r="M92" s="147"/>
+      <c r="N92" s="147"/>
+      <c r="O92" s="147"/>
+      <c r="P92" s="147"/>
+      <c r="Q92" s="147"/>
+      <c r="R92" s="147"/>
+      <c r="S92" s="147"/>
+      <c r="T92" s="147"/>
+      <c r="U92" s="147"/>
+      <c r="V92" s="147"/>
+      <c r="W92" s="153"/>
     </row>
     <row r="93" spans="1:23" ht="12" customHeight="1">
       <c r="A93" s="122"/>
@@ -4411,31 +4411,31 @@
       <c r="T93" s="90"/>
       <c r="U93" s="90"/>
       <c r="V93" s="90"/>
-      <c r="W93" s="139"/>
+      <c r="W93" s="132"/>
     </row>
     <row r="94" spans="1:23" ht="12" customHeight="1">
       <c r="A94" s="122"/>
       <c r="B94" s="122"/>
-      <c r="C94" s="170"/>
-      <c r="D94" s="171"/>
+      <c r="C94" s="169"/>
+      <c r="D94" s="170"/>
       <c r="E94" s="37"/>
       <c r="F94" s="59"/>
       <c r="G94" s="55"/>
       <c r="H94" s="55"/>
       <c r="I94" s="111"/>
-      <c r="J94" s="164"/>
-      <c r="K94" s="165"/>
-      <c r="L94" s="141"/>
-      <c r="M94" s="141"/>
-      <c r="N94" s="141"/>
-      <c r="O94" s="141"/>
-      <c r="P94" s="141"/>
-      <c r="Q94" s="141"/>
-      <c r="R94" s="141"/>
-      <c r="S94" s="141"/>
-      <c r="T94" s="141"/>
-      <c r="U94" s="141"/>
-      <c r="V94" s="141"/>
+      <c r="J94" s="163"/>
+      <c r="K94" s="164"/>
+      <c r="L94" s="140"/>
+      <c r="M94" s="140"/>
+      <c r="N94" s="140"/>
+      <c r="O94" s="140"/>
+      <c r="P94" s="140"/>
+      <c r="Q94" s="140"/>
+      <c r="R94" s="140"/>
+      <c r="S94" s="140"/>
+      <c r="T94" s="140"/>
+      <c r="U94" s="140"/>
+      <c r="V94" s="140"/>
       <c r="W94" s="135"/>
     </row>
     <row r="95" spans="1:23" ht="12" customHeight="1">
@@ -4473,20 +4473,20 @@
       <c r="G96" s="61"/>
       <c r="H96" s="62"/>
       <c r="I96" s="100"/>
-      <c r="J96" s="162"/>
-      <c r="K96" s="163"/>
-      <c r="L96" s="148"/>
-      <c r="M96" s="148"/>
-      <c r="N96" s="148"/>
-      <c r="O96" s="148"/>
-      <c r="P96" s="148"/>
-      <c r="Q96" s="148"/>
-      <c r="R96" s="148"/>
-      <c r="S96" s="148"/>
-      <c r="T96" s="148"/>
-      <c r="U96" s="148"/>
-      <c r="V96" s="148"/>
-      <c r="W96" s="133"/>
+      <c r="J96" s="161"/>
+      <c r="K96" s="162"/>
+      <c r="L96" s="147"/>
+      <c r="M96" s="147"/>
+      <c r="N96" s="147"/>
+      <c r="O96" s="147"/>
+      <c r="P96" s="147"/>
+      <c r="Q96" s="147"/>
+      <c r="R96" s="147"/>
+      <c r="S96" s="147"/>
+      <c r="T96" s="147"/>
+      <c r="U96" s="147"/>
+      <c r="V96" s="147"/>
+      <c r="W96" s="153"/>
     </row>
     <row r="97" spans="1:23" ht="12" customHeight="1">
       <c r="A97" s="121"/>
@@ -4511,31 +4511,10 @@
       <c r="T97" s="90"/>
       <c r="U97" s="90"/>
       <c r="V97" s="90"/>
-      <c r="W97" s="139"/>
+      <c r="W97" s="181"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A6:W6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C46:D46"/>
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C94:D94"/>
@@ -4545,6 +4524,27 @@
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A6:W6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix bug kdr001 #  #118769
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
@@ -1706,29 +1706,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1753,6 +1735,24 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="76" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1799,7 +1799,7 @@
         <xdr:cNvPr id="2" name="楕円 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -45114,37 +45114,37 @@
     <col min="4" max="4" width="10.6640625" style="140" customWidth="1"/>
     <col min="5" max="9" width="5.6640625" style="140"/>
     <col min="10" max="10" width="6.6640625" style="140" customWidth="1"/>
-    <col min="11" max="11" width="5.33203125" style="26" customWidth="1"/>
-    <col min="12" max="22" width="5.6640625" style="26"/>
-    <col min="23" max="24" width="5.6640625" style="25"/>
+    <col min="11" max="22" width="5.33203125" style="26" customWidth="1"/>
+    <col min="23" max="23" width="4.83203125" style="25" customWidth="1"/>
+    <col min="24" max="24" width="5.6640625" style="25"/>
     <col min="25" max="16384" width="5.6640625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="0.75" customHeight="1"/>
     <row r="2" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A2" s="174"/>
-      <c r="B2" s="174"/>
-      <c r="C2" s="174"/>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="174"/>
-      <c r="K2" s="174"/>
-      <c r="L2" s="174"/>
-      <c r="M2" s="174"/>
-      <c r="N2" s="174"/>
-      <c r="O2" s="174"/>
-      <c r="P2" s="174"/>
-      <c r="Q2" s="174"/>
-      <c r="R2" s="174"/>
-      <c r="S2" s="174"/>
-      <c r="T2" s="174"/>
-      <c r="U2" s="174"/>
-      <c r="V2" s="174"/>
-      <c r="W2" s="174"/>
+      <c r="A2" s="168"/>
+      <c r="B2" s="168"/>
+      <c r="C2" s="168"/>
+      <c r="D2" s="168"/>
+      <c r="E2" s="168"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="168"/>
+      <c r="H2" s="168"/>
+      <c r="I2" s="168"/>
+      <c r="J2" s="168"/>
+      <c r="K2" s="168"/>
+      <c r="L2" s="168"/>
+      <c r="M2" s="168"/>
+      <c r="N2" s="168"/>
+      <c r="O2" s="168"/>
+      <c r="P2" s="168"/>
+      <c r="Q2" s="168"/>
+      <c r="R2" s="168"/>
+      <c r="S2" s="168"/>
+      <c r="T2" s="168"/>
+      <c r="U2" s="168"/>
+      <c r="V2" s="168"/>
+      <c r="W2" s="168"/>
     </row>
     <row r="3" spans="1:23" ht="0.75" customHeight="1" thickBot="1">
       <c r="A3" s="27"/>
@@ -45176,13 +45176,13 @@
       <c r="B4" s="28"/>
       <c r="C4" s="29"/>
       <c r="D4" s="28"/>
-      <c r="E4" s="175"/>
-      <c r="F4" s="176"/>
-      <c r="G4" s="176"/>
-      <c r="H4" s="176"/>
-      <c r="I4" s="177"/>
-      <c r="J4" s="178"/>
-      <c r="K4" s="176"/>
+      <c r="E4" s="169"/>
+      <c r="F4" s="170"/>
+      <c r="G4" s="170"/>
+      <c r="H4" s="170"/>
+      <c r="I4" s="171"/>
+      <c r="J4" s="172"/>
+      <c r="K4" s="170"/>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
@@ -45222,33 +45222,33 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A6" s="179"/>
-      <c r="B6" s="179"/>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
-      <c r="G6" s="179"/>
-      <c r="H6" s="179"/>
-      <c r="I6" s="179"/>
-      <c r="J6" s="179"/>
-      <c r="K6" s="179"/>
-      <c r="L6" s="179"/>
-      <c r="M6" s="179"/>
-      <c r="N6" s="179"/>
-      <c r="O6" s="179"/>
-      <c r="P6" s="179"/>
-      <c r="Q6" s="179"/>
-      <c r="R6" s="179"/>
-      <c r="S6" s="179"/>
-      <c r="T6" s="179"/>
-      <c r="U6" s="179"/>
-      <c r="V6" s="179"/>
-      <c r="W6" s="179"/>
+      <c r="A6" s="173"/>
+      <c r="B6" s="173"/>
+      <c r="C6" s="173"/>
+      <c r="D6" s="173"/>
+      <c r="E6" s="173"/>
+      <c r="F6" s="173"/>
+      <c r="G6" s="173"/>
+      <c r="H6" s="173"/>
+      <c r="I6" s="173"/>
+      <c r="J6" s="173"/>
+      <c r="K6" s="173"/>
+      <c r="L6" s="173"/>
+      <c r="M6" s="173"/>
+      <c r="N6" s="173"/>
+      <c r="O6" s="173"/>
+      <c r="P6" s="173"/>
+      <c r="Q6" s="173"/>
+      <c r="R6" s="173"/>
+      <c r="S6" s="173"/>
+      <c r="T6" s="173"/>
+      <c r="U6" s="173"/>
+      <c r="V6" s="173"/>
+      <c r="W6" s="173"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
-      <c r="A7" s="180"/>
-      <c r="B7" s="181"/>
+      <c r="A7" s="174"/>
+      <c r="B7" s="175"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
@@ -45272,8 +45272,8 @@
       <c r="W7" s="40"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="170"/>
-      <c r="B8" s="171"/>
+      <c r="A8" s="176"/>
+      <c r="B8" s="177"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -45297,8 +45297,8 @@
       <c r="W8" s="45"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
-      <c r="A9" s="172"/>
-      <c r="B9" s="173"/>
+      <c r="A9" s="178"/>
+      <c r="B9" s="179"/>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -45322,8 +45322,8 @@
       <c r="W9" s="52"/>
     </row>
     <row r="10" spans="1:23" ht="12" customHeight="1">
-      <c r="A10" s="170"/>
-      <c r="B10" s="171"/>
+      <c r="A10" s="176"/>
+      <c r="B10" s="177"/>
       <c r="C10" s="4"/>
       <c r="D10" s="9"/>
       <c r="E10" s="6"/>
@@ -45347,8 +45347,8 @@
       <c r="W10" s="45"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
-      <c r="A11" s="170"/>
-      <c r="B11" s="171"/>
+      <c r="A11" s="176"/>
+      <c r="B11" s="177"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="10"/>
@@ -45399,8 +45399,8 @@
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="164"/>
       <c r="B13" s="164"/>
-      <c r="C13" s="168"/>
-      <c r="D13" s="169"/>
+      <c r="C13" s="166"/>
+      <c r="D13" s="167"/>
       <c r="E13" s="63"/>
       <c r="F13" s="64"/>
       <c r="G13" s="64"/>
@@ -45449,8 +45449,8 @@
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="166"/>
-      <c r="D15" s="167"/>
+      <c r="C15" s="180"/>
+      <c r="D15" s="181"/>
       <c r="E15" s="71"/>
       <c r="F15" s="72"/>
       <c r="G15" s="72"/>
@@ -45474,8 +45474,8 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="168"/>
-      <c r="D16" s="169"/>
+      <c r="C16" s="166"/>
+      <c r="D16" s="167"/>
       <c r="E16" s="63"/>
       <c r="F16" s="64"/>
       <c r="G16" s="64"/>
@@ -45524,8 +45524,8 @@
     <row r="18" spans="1:23" ht="12" customHeight="1">
       <c r="A18" s="164"/>
       <c r="B18" s="164"/>
-      <c r="C18" s="168"/>
-      <c r="D18" s="169"/>
+      <c r="C18" s="166"/>
+      <c r="D18" s="167"/>
       <c r="E18" s="87"/>
       <c r="F18" s="88"/>
       <c r="G18" s="88"/>
@@ -45624,8 +45624,8 @@
     <row r="22" spans="1:23" ht="12" customHeight="1">
       <c r="A22" s="164"/>
       <c r="B22" s="164"/>
-      <c r="C22" s="168"/>
-      <c r="D22" s="169"/>
+      <c r="C22" s="166"/>
+      <c r="D22" s="167"/>
       <c r="E22" s="87"/>
       <c r="F22" s="88"/>
       <c r="G22" s="88"/>
@@ -45724,8 +45724,8 @@
     <row r="26" spans="1:23" ht="12" customHeight="1">
       <c r="A26" s="164"/>
       <c r="B26" s="164"/>
-      <c r="C26" s="168"/>
-      <c r="D26" s="169"/>
+      <c r="C26" s="166"/>
+      <c r="D26" s="167"/>
       <c r="E26" s="87"/>
       <c r="F26" s="88"/>
       <c r="G26" s="88"/>
@@ -45824,8 +45824,8 @@
     <row r="30" spans="1:23" ht="12" customHeight="1">
       <c r="A30" s="164"/>
       <c r="B30" s="164"/>
-      <c r="C30" s="168"/>
-      <c r="D30" s="169"/>
+      <c r="C30" s="166"/>
+      <c r="D30" s="167"/>
       <c r="E30" s="107"/>
       <c r="F30" s="88"/>
       <c r="G30" s="88"/>
@@ -45924,8 +45924,8 @@
     <row r="34" spans="1:23" ht="12" customHeight="1">
       <c r="A34" s="164"/>
       <c r="B34" s="164"/>
-      <c r="C34" s="168"/>
-      <c r="D34" s="169"/>
+      <c r="C34" s="166"/>
+      <c r="D34" s="167"/>
       <c r="E34" s="113"/>
       <c r="F34" s="114"/>
       <c r="G34" s="88"/>
@@ -46024,8 +46024,8 @@
     <row r="38" spans="1:23" ht="12" customHeight="1">
       <c r="A38" s="164"/>
       <c r="B38" s="164"/>
-      <c r="C38" s="168"/>
-      <c r="D38" s="169"/>
+      <c r="C38" s="166"/>
+      <c r="D38" s="167"/>
       <c r="E38" s="127"/>
       <c r="F38" s="66"/>
       <c r="G38" s="66"/>
@@ -46124,8 +46124,8 @@
     <row r="42" spans="1:23" ht="12" customHeight="1">
       <c r="A42" s="164"/>
       <c r="B42" s="164"/>
-      <c r="C42" s="168"/>
-      <c r="D42" s="169"/>
+      <c r="C42" s="166"/>
+      <c r="D42" s="167"/>
       <c r="E42" s="127"/>
       <c r="F42" s="66"/>
       <c r="G42" s="66"/>
@@ -46224,8 +46224,8 @@
     <row r="46" spans="1:23" ht="12" customHeight="1">
       <c r="A46" s="164"/>
       <c r="B46" s="164"/>
-      <c r="C46" s="168"/>
-      <c r="D46" s="169"/>
+      <c r="C46" s="166"/>
+      <c r="D46" s="167"/>
       <c r="E46" s="87"/>
       <c r="F46" s="131"/>
       <c r="G46" s="66"/>
@@ -46324,8 +46324,8 @@
     <row r="50" spans="1:23" ht="12" customHeight="1">
       <c r="A50" s="164"/>
       <c r="B50" s="164"/>
-      <c r="C50" s="168"/>
-      <c r="D50" s="169"/>
+      <c r="C50" s="166"/>
+      <c r="D50" s="167"/>
       <c r="E50" s="87"/>
       <c r="F50" s="131"/>
       <c r="G50" s="66"/>
@@ -46583,8 +46583,8 @@
       <c r="W61" s="144"/>
     </row>
     <row r="64" spans="1:23" ht="12" customHeight="1">
-      <c r="C64" s="168"/>
-      <c r="D64" s="169"/>
+      <c r="C64" s="166"/>
+      <c r="D64" s="167"/>
       <c r="E64" s="63"/>
       <c r="F64" s="64"/>
       <c r="G64" s="64"/>
@@ -46631,8 +46631,8 @@
     <row r="66" spans="1:23" ht="12" customHeight="1">
       <c r="A66" s="164"/>
       <c r="B66" s="164"/>
-      <c r="C66" s="168"/>
-      <c r="D66" s="169"/>
+      <c r="C66" s="166"/>
+      <c r="D66" s="167"/>
       <c r="E66" s="87"/>
       <c r="F66" s="88"/>
       <c r="G66" s="88"/>
@@ -46731,8 +46731,8 @@
     <row r="70" spans="1:23" ht="12" customHeight="1">
       <c r="A70" s="164"/>
       <c r="B70" s="164"/>
-      <c r="C70" s="168"/>
-      <c r="D70" s="169"/>
+      <c r="C70" s="166"/>
+      <c r="D70" s="167"/>
       <c r="E70" s="87"/>
       <c r="F70" s="88"/>
       <c r="G70" s="88"/>
@@ -46831,8 +46831,8 @@
     <row r="74" spans="1:23" ht="12" customHeight="1">
       <c r="A74" s="164"/>
       <c r="B74" s="164"/>
-      <c r="C74" s="168"/>
-      <c r="D74" s="169"/>
+      <c r="C74" s="166"/>
+      <c r="D74" s="167"/>
       <c r="E74" s="107"/>
       <c r="F74" s="88"/>
       <c r="G74" s="88"/>
@@ -46931,8 +46931,8 @@
     <row r="78" spans="1:23" ht="12" customHeight="1">
       <c r="A78" s="164"/>
       <c r="B78" s="164"/>
-      <c r="C78" s="168"/>
-      <c r="D78" s="169"/>
+      <c r="C78" s="166"/>
+      <c r="D78" s="167"/>
       <c r="E78" s="113"/>
       <c r="F78" s="114"/>
       <c r="G78" s="88"/>
@@ -47031,8 +47031,8 @@
     <row r="82" spans="1:23" ht="12" customHeight="1">
       <c r="A82" s="164"/>
       <c r="B82" s="164"/>
-      <c r="C82" s="168"/>
-      <c r="D82" s="169"/>
+      <c r="C82" s="166"/>
+      <c r="D82" s="167"/>
       <c r="E82" s="127"/>
       <c r="F82" s="66"/>
       <c r="G82" s="66"/>
@@ -47131,8 +47131,8 @@
     <row r="86" spans="1:23" ht="12" customHeight="1">
       <c r="A86" s="164"/>
       <c r="B86" s="164"/>
-      <c r="C86" s="168"/>
-      <c r="D86" s="169"/>
+      <c r="C86" s="166"/>
+      <c r="D86" s="167"/>
       <c r="E86" s="127"/>
       <c r="F86" s="66"/>
       <c r="G86" s="66"/>
@@ -47231,8 +47231,8 @@
     <row r="90" spans="1:23" ht="12" customHeight="1">
       <c r="A90" s="164"/>
       <c r="B90" s="164"/>
-      <c r="C90" s="168"/>
-      <c r="D90" s="169"/>
+      <c r="C90" s="166"/>
+      <c r="D90" s="167"/>
       <c r="E90" s="87"/>
       <c r="F90" s="131"/>
       <c r="G90" s="66"/>
@@ -47331,8 +47331,8 @@
     <row r="94" spans="1:23" ht="12" customHeight="1">
       <c r="A94" s="164"/>
       <c r="B94" s="164"/>
-      <c r="C94" s="168"/>
-      <c r="D94" s="169"/>
+      <c r="C94" s="166"/>
+      <c r="D94" s="167"/>
       <c r="E94" s="87"/>
       <c r="F94" s="131"/>
       <c r="G94" s="66"/>
@@ -47433,6 +47433,27 @@
     </row>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A6:W6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="C34:D34"/>
+    <mergeCell ref="C38:D38"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="C46:D46"/>
     <mergeCell ref="C86:D86"/>
     <mergeCell ref="C90:D90"/>
     <mergeCell ref="C94:D94"/>
@@ -47442,27 +47463,6 @@
     <mergeCell ref="C78:D78"/>
     <mergeCell ref="C82:D82"/>
     <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A6:W6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C26:D26"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>

<commit_message>
fix bug kdr001 # 118790
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
@@ -185,7 +185,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="81">
+  <borders count="82">
     <border>
       <left/>
       <right/>
@@ -1199,6 +1199,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dashed">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1207,7 +1220,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="182">
+  <cellXfs count="187">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1706,6 +1719,15 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1753,6 +1775,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="5" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -45122,29 +45150,29 @@
   <sheetData>
     <row r="1" spans="1:23" ht="0.75" customHeight="1"/>
     <row r="2" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A2" s="168"/>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
+      <c r="A2" s="171"/>
+      <c r="B2" s="171"/>
+      <c r="C2" s="171"/>
+      <c r="D2" s="171"/>
+      <c r="E2" s="171"/>
+      <c r="F2" s="171"/>
+      <c r="G2" s="171"/>
+      <c r="H2" s="171"/>
+      <c r="I2" s="171"/>
+      <c r="J2" s="171"/>
+      <c r="K2" s="171"/>
+      <c r="L2" s="171"/>
+      <c r="M2" s="171"/>
+      <c r="N2" s="171"/>
+      <c r="O2" s="171"/>
+      <c r="P2" s="171"/>
+      <c r="Q2" s="171"/>
+      <c r="R2" s="171"/>
+      <c r="S2" s="171"/>
+      <c r="T2" s="171"/>
+      <c r="U2" s="171"/>
+      <c r="V2" s="171"/>
+      <c r="W2" s="171"/>
     </row>
     <row r="3" spans="1:23" ht="0.75" customHeight="1" thickBot="1">
       <c r="A3" s="27"/>
@@ -45176,13 +45204,13 @@
       <c r="B4" s="28"/>
       <c r="C4" s="29"/>
       <c r="D4" s="28"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="170"/>
-      <c r="G4" s="170"/>
-      <c r="H4" s="170"/>
-      <c r="I4" s="171"/>
-      <c r="J4" s="172"/>
-      <c r="K4" s="170"/>
+      <c r="E4" s="172"/>
+      <c r="F4" s="173"/>
+      <c r="G4" s="173"/>
+      <c r="H4" s="173"/>
+      <c r="I4" s="174"/>
+      <c r="J4" s="175"/>
+      <c r="K4" s="173"/>
       <c r="L4" s="28"/>
       <c r="M4" s="28"/>
       <c r="N4" s="28"/>
@@ -45222,33 +45250,33 @@
       <c r="W5" s="22"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A6" s="173"/>
-      <c r="B6" s="173"/>
-      <c r="C6" s="173"/>
-      <c r="D6" s="173"/>
-      <c r="E6" s="173"/>
-      <c r="F6" s="173"/>
-      <c r="G6" s="173"/>
-      <c r="H6" s="173"/>
-      <c r="I6" s="173"/>
-      <c r="J6" s="173"/>
-      <c r="K6" s="173"/>
-      <c r="L6" s="173"/>
-      <c r="M6" s="173"/>
-      <c r="N6" s="173"/>
-      <c r="O6" s="173"/>
-      <c r="P6" s="173"/>
-      <c r="Q6" s="173"/>
-      <c r="R6" s="173"/>
-      <c r="S6" s="173"/>
-      <c r="T6" s="173"/>
-      <c r="U6" s="173"/>
-      <c r="V6" s="173"/>
-      <c r="W6" s="173"/>
+      <c r="A6" s="176"/>
+      <c r="B6" s="176"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176"/>
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="176"/>
+      <c r="K6" s="176"/>
+      <c r="L6" s="176"/>
+      <c r="M6" s="176"/>
+      <c r="N6" s="176"/>
+      <c r="O6" s="176"/>
+      <c r="P6" s="176"/>
+      <c r="Q6" s="176"/>
+      <c r="R6" s="176"/>
+      <c r="S6" s="176"/>
+      <c r="T6" s="176"/>
+      <c r="U6" s="176"/>
+      <c r="V6" s="176"/>
+      <c r="W6" s="176"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
-      <c r="A7" s="174"/>
-      <c r="B7" s="175"/>
+      <c r="A7" s="177"/>
+      <c r="B7" s="178"/>
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
       <c r="E7" s="3"/>
@@ -45272,8 +45300,8 @@
       <c r="W7" s="40"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="176"/>
-      <c r="B8" s="177"/>
+      <c r="A8" s="179"/>
+      <c r="B8" s="180"/>
       <c r="C8" s="4"/>
       <c r="D8" s="5"/>
       <c r="E8" s="6"/>
@@ -45297,8 +45325,8 @@
       <c r="W8" s="45"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
-      <c r="A9" s="178"/>
-      <c r="B9" s="179"/>
+      <c r="A9" s="181"/>
+      <c r="B9" s="182"/>
       <c r="C9" s="4"/>
       <c r="D9" s="7"/>
       <c r="E9" s="8"/>
@@ -45322,8 +45350,8 @@
       <c r="W9" s="52"/>
     </row>
     <row r="10" spans="1:23" ht="12" customHeight="1">
-      <c r="A10" s="176"/>
-      <c r="B10" s="177"/>
+      <c r="A10" s="179"/>
+      <c r="B10" s="180"/>
       <c r="C10" s="4"/>
       <c r="D10" s="9"/>
       <c r="E10" s="6"/>
@@ -45347,8 +45375,8 @@
       <c r="W10" s="45"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
-      <c r="A11" s="176"/>
-      <c r="B11" s="177"/>
+      <c r="A11" s="179"/>
+      <c r="B11" s="180"/>
       <c r="C11" s="4"/>
       <c r="D11" s="5"/>
       <c r="E11" s="10"/>
@@ -45399,8 +45427,8 @@
     <row r="13" spans="1:23" ht="12" customHeight="1">
       <c r="A13" s="164"/>
       <c r="B13" s="164"/>
-      <c r="C13" s="166"/>
-      <c r="D13" s="167"/>
+      <c r="C13" s="169"/>
+      <c r="D13" s="170"/>
       <c r="E13" s="63"/>
       <c r="F13" s="64"/>
       <c r="G13" s="64"/>
@@ -45449,8 +45477,8 @@
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="25"/>
       <c r="B15" s="25"/>
-      <c r="C15" s="180"/>
-      <c r="D15" s="181"/>
+      <c r="C15" s="183"/>
+      <c r="D15" s="184"/>
       <c r="E15" s="71"/>
       <c r="F15" s="72"/>
       <c r="G15" s="72"/>
@@ -45474,8 +45502,8 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="25"/>
       <c r="B16" s="25"/>
-      <c r="C16" s="166"/>
-      <c r="D16" s="167"/>
+      <c r="C16" s="169"/>
+      <c r="D16" s="170"/>
       <c r="E16" s="63"/>
       <c r="F16" s="64"/>
       <c r="G16" s="64"/>
@@ -45524,8 +45552,8 @@
     <row r="18" spans="1:23" ht="12" customHeight="1">
       <c r="A18" s="164"/>
       <c r="B18" s="164"/>
-      <c r="C18" s="166"/>
-      <c r="D18" s="167"/>
+      <c r="C18" s="169"/>
+      <c r="D18" s="170"/>
       <c r="E18" s="87"/>
       <c r="F18" s="88"/>
       <c r="G18" s="88"/>
@@ -45624,8 +45652,8 @@
     <row r="22" spans="1:23" ht="12" customHeight="1">
       <c r="A22" s="164"/>
       <c r="B22" s="164"/>
-      <c r="C22" s="166"/>
-      <c r="D22" s="167"/>
+      <c r="C22" s="169"/>
+      <c r="D22" s="170"/>
       <c r="E22" s="87"/>
       <c r="F22" s="88"/>
       <c r="G22" s="88"/>
@@ -45724,14 +45752,14 @@
     <row r="26" spans="1:23" ht="12" customHeight="1">
       <c r="A26" s="164"/>
       <c r="B26" s="164"/>
-      <c r="C26" s="166"/>
-      <c r="D26" s="167"/>
+      <c r="C26" s="169"/>
+      <c r="D26" s="170"/>
       <c r="E26" s="87"/>
       <c r="F26" s="88"/>
       <c r="G26" s="88"/>
       <c r="H26" s="88"/>
       <c r="I26" s="105"/>
-      <c r="J26" s="81"/>
+      <c r="J26" s="167"/>
       <c r="K26" s="82"/>
       <c r="L26" s="83"/>
       <c r="M26" s="83"/>
@@ -45781,7 +45809,7 @@
       <c r="G28" s="97"/>
       <c r="H28" s="97"/>
       <c r="I28" s="98"/>
-      <c r="J28" s="106"/>
+      <c r="J28" s="168"/>
       <c r="K28" s="53"/>
       <c r="L28" s="100"/>
       <c r="M28" s="100"/>
@@ -45806,7 +45834,7 @@
       <c r="G29" s="103"/>
       <c r="H29" s="103"/>
       <c r="I29" s="104"/>
-      <c r="J29" s="86"/>
+      <c r="J29" s="185"/>
       <c r="K29" s="51"/>
       <c r="L29" s="50"/>
       <c r="M29" s="50"/>
@@ -45824,8 +45852,8 @@
     <row r="30" spans="1:23" ht="12" customHeight="1">
       <c r="A30" s="164"/>
       <c r="B30" s="164"/>
-      <c r="C30" s="166"/>
-      <c r="D30" s="167"/>
+      <c r="C30" s="169"/>
+      <c r="D30" s="170"/>
       <c r="E30" s="107"/>
       <c r="F30" s="88"/>
       <c r="G30" s="88"/>
@@ -45924,8 +45952,8 @@
     <row r="34" spans="1:23" ht="12" customHeight="1">
       <c r="A34" s="164"/>
       <c r="B34" s="164"/>
-      <c r="C34" s="166"/>
-      <c r="D34" s="167"/>
+      <c r="C34" s="169"/>
+      <c r="D34" s="170"/>
       <c r="E34" s="113"/>
       <c r="F34" s="114"/>
       <c r="G34" s="88"/>
@@ -46024,14 +46052,14 @@
     <row r="38" spans="1:23" ht="12" customHeight="1">
       <c r="A38" s="164"/>
       <c r="B38" s="164"/>
-      <c r="C38" s="166"/>
-      <c r="D38" s="167"/>
+      <c r="C38" s="169"/>
+      <c r="D38" s="170"/>
       <c r="E38" s="127"/>
       <c r="F38" s="66"/>
       <c r="G38" s="66"/>
       <c r="H38" s="66"/>
       <c r="I38" s="108"/>
-      <c r="J38" s="81"/>
+      <c r="J38" s="167"/>
       <c r="K38" s="82"/>
       <c r="L38" s="83"/>
       <c r="M38" s="83"/>
@@ -46081,7 +46109,7 @@
       <c r="G40" s="97"/>
       <c r="H40" s="129"/>
       <c r="I40" s="110"/>
-      <c r="J40" s="106"/>
+      <c r="J40" s="168"/>
       <c r="K40" s="53"/>
       <c r="L40" s="100"/>
       <c r="M40" s="100"/>
@@ -46106,7 +46134,7 @@
       <c r="G41" s="103"/>
       <c r="H41" s="130"/>
       <c r="I41" s="112"/>
-      <c r="J41" s="86"/>
+      <c r="J41" s="166"/>
       <c r="K41" s="51"/>
       <c r="L41" s="50"/>
       <c r="M41" s="50"/>
@@ -46124,14 +46152,14 @@
     <row r="42" spans="1:23" ht="12" customHeight="1">
       <c r="A42" s="164"/>
       <c r="B42" s="164"/>
-      <c r="C42" s="166"/>
-      <c r="D42" s="167"/>
+      <c r="C42" s="169"/>
+      <c r="D42" s="170"/>
       <c r="E42" s="127"/>
       <c r="F42" s="66"/>
       <c r="G42" s="66"/>
       <c r="H42" s="66"/>
       <c r="I42" s="108"/>
-      <c r="J42" s="81"/>
+      <c r="J42" s="167"/>
       <c r="K42" s="82"/>
       <c r="L42" s="83"/>
       <c r="M42" s="83"/>
@@ -46181,7 +46209,7 @@
       <c r="G44" s="97"/>
       <c r="H44" s="129"/>
       <c r="I44" s="110"/>
-      <c r="J44" s="106"/>
+      <c r="J44" s="168"/>
       <c r="K44" s="53"/>
       <c r="L44" s="100"/>
       <c r="M44" s="100"/>
@@ -46206,7 +46234,7 @@
       <c r="G45" s="103"/>
       <c r="H45" s="103"/>
       <c r="I45" s="112"/>
-      <c r="J45" s="86"/>
+      <c r="J45" s="166"/>
       <c r="K45" s="51"/>
       <c r="L45" s="50"/>
       <c r="M45" s="50"/>
@@ -46224,14 +46252,14 @@
     <row r="46" spans="1:23" ht="12" customHeight="1">
       <c r="A46" s="164"/>
       <c r="B46" s="164"/>
-      <c r="C46" s="166"/>
-      <c r="D46" s="167"/>
+      <c r="C46" s="169"/>
+      <c r="D46" s="170"/>
       <c r="E46" s="87"/>
       <c r="F46" s="131"/>
       <c r="G46" s="66"/>
       <c r="H46" s="66"/>
       <c r="I46" s="132"/>
-      <c r="J46" s="81"/>
+      <c r="J46" s="167"/>
       <c r="K46" s="82"/>
       <c r="L46" s="83"/>
       <c r="M46" s="83"/>
@@ -46281,7 +46309,7 @@
       <c r="G48" s="134"/>
       <c r="H48" s="135"/>
       <c r="I48" s="110"/>
-      <c r="J48" s="106"/>
+      <c r="J48" s="186"/>
       <c r="K48" s="53"/>
       <c r="L48" s="100"/>
       <c r="M48" s="100"/>
@@ -46306,7 +46334,7 @@
       <c r="G49" s="102"/>
       <c r="H49" s="130"/>
       <c r="I49" s="112"/>
-      <c r="J49" s="86"/>
+      <c r="J49" s="185"/>
       <c r="K49" s="51"/>
       <c r="L49" s="50"/>
       <c r="M49" s="50"/>
@@ -46324,14 +46352,14 @@
     <row r="50" spans="1:23" ht="12" customHeight="1">
       <c r="A50" s="164"/>
       <c r="B50" s="164"/>
-      <c r="C50" s="166"/>
-      <c r="D50" s="167"/>
+      <c r="C50" s="169"/>
+      <c r="D50" s="170"/>
       <c r="E50" s="87"/>
       <c r="F50" s="131"/>
       <c r="G50" s="66"/>
       <c r="H50" s="66"/>
       <c r="I50" s="132"/>
-      <c r="J50" s="81"/>
+      <c r="J50" s="167"/>
       <c r="K50" s="82"/>
       <c r="L50" s="83"/>
       <c r="M50" s="83"/>
@@ -46381,7 +46409,7 @@
       <c r="G52" s="134"/>
       <c r="H52" s="135"/>
       <c r="I52" s="110"/>
-      <c r="J52" s="106"/>
+      <c r="J52" s="186"/>
       <c r="K52" s="53"/>
       <c r="L52" s="100"/>
       <c r="M52" s="100"/>
@@ -46406,7 +46434,7 @@
       <c r="G53" s="102"/>
       <c r="H53" s="130"/>
       <c r="I53" s="112"/>
-      <c r="J53" s="76"/>
+      <c r="J53" s="185"/>
       <c r="K53" s="137"/>
       <c r="L53" s="138"/>
       <c r="M53" s="138"/>
@@ -46583,8 +46611,8 @@
       <c r="W61" s="144"/>
     </row>
     <row r="64" spans="1:23" ht="12" customHeight="1">
-      <c r="C64" s="166"/>
-      <c r="D64" s="167"/>
+      <c r="C64" s="169"/>
+      <c r="D64" s="170"/>
       <c r="E64" s="63"/>
       <c r="F64" s="64"/>
       <c r="G64" s="64"/>
@@ -46631,8 +46659,8 @@
     <row r="66" spans="1:23" ht="12" customHeight="1">
       <c r="A66" s="164"/>
       <c r="B66" s="164"/>
-      <c r="C66" s="166"/>
-      <c r="D66" s="167"/>
+      <c r="C66" s="169"/>
+      <c r="D66" s="170"/>
       <c r="E66" s="87"/>
       <c r="F66" s="88"/>
       <c r="G66" s="88"/>
@@ -46731,8 +46759,8 @@
     <row r="70" spans="1:23" ht="12" customHeight="1">
       <c r="A70" s="164"/>
       <c r="B70" s="164"/>
-      <c r="C70" s="166"/>
-      <c r="D70" s="167"/>
+      <c r="C70" s="169"/>
+      <c r="D70" s="170"/>
       <c r="E70" s="87"/>
       <c r="F70" s="88"/>
       <c r="G70" s="88"/>
@@ -46831,8 +46859,8 @@
     <row r="74" spans="1:23" ht="12" customHeight="1">
       <c r="A74" s="164"/>
       <c r="B74" s="164"/>
-      <c r="C74" s="166"/>
-      <c r="D74" s="167"/>
+      <c r="C74" s="169"/>
+      <c r="D74" s="170"/>
       <c r="E74" s="107"/>
       <c r="F74" s="88"/>
       <c r="G74" s="88"/>
@@ -46931,8 +46959,8 @@
     <row r="78" spans="1:23" ht="12" customHeight="1">
       <c r="A78" s="164"/>
       <c r="B78" s="164"/>
-      <c r="C78" s="166"/>
-      <c r="D78" s="167"/>
+      <c r="C78" s="169"/>
+      <c r="D78" s="170"/>
       <c r="E78" s="113"/>
       <c r="F78" s="114"/>
       <c r="G78" s="88"/>
@@ -47031,8 +47059,8 @@
     <row r="82" spans="1:23" ht="12" customHeight="1">
       <c r="A82" s="164"/>
       <c r="B82" s="164"/>
-      <c r="C82" s="166"/>
-      <c r="D82" s="167"/>
+      <c r="C82" s="169"/>
+      <c r="D82" s="170"/>
       <c r="E82" s="127"/>
       <c r="F82" s="66"/>
       <c r="G82" s="66"/>
@@ -47131,8 +47159,8 @@
     <row r="86" spans="1:23" ht="12" customHeight="1">
       <c r="A86" s="164"/>
       <c r="B86" s="164"/>
-      <c r="C86" s="166"/>
-      <c r="D86" s="167"/>
+      <c r="C86" s="169"/>
+      <c r="D86" s="170"/>
       <c r="E86" s="127"/>
       <c r="F86" s="66"/>
       <c r="G86" s="66"/>
@@ -47231,8 +47259,8 @@
     <row r="90" spans="1:23" ht="12" customHeight="1">
       <c r="A90" s="164"/>
       <c r="B90" s="164"/>
-      <c r="C90" s="166"/>
-      <c r="D90" s="167"/>
+      <c r="C90" s="169"/>
+      <c r="D90" s="170"/>
       <c r="E90" s="87"/>
       <c r="F90" s="131"/>
       <c r="G90" s="66"/>
@@ -47331,8 +47359,8 @@
     <row r="94" spans="1:23" ht="12" customHeight="1">
       <c r="A94" s="164"/>
       <c r="B94" s="164"/>
-      <c r="C94" s="166"/>
-      <c r="D94" s="167"/>
+      <c r="C94" s="169"/>
+      <c r="D94" s="170"/>
       <c r="E94" s="87"/>
       <c r="F94" s="131"/>
       <c r="G94" s="66"/>

</xml_diff>

<commit_message>
fix bug kdr001 # 56202
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
+++ b/nts.uk/uk.at/at.ctx/function/nts.uk.ctx.at.function.infra/src/main/resources/report/KDR001_v2_template.xlsx
@@ -1227,7 +1227,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="190">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1711,9 +1711,6 @@
     <xf numFmtId="49" fontId="1" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="5" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
@@ -1729,26 +1726,38 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="21" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="76" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
@@ -1762,11 +1771,11 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="78" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
@@ -1774,28 +1783,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="76" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
@@ -1843,7 +1840,7 @@
         <xdr:cNvPr id="2" name="楕円 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -45157,7 +45154,7 @@
     <col min="3" max="3" width="3.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="10.6640625" style="1" customWidth="1"/>
     <col min="5" max="9" width="5.6640625" style="1"/>
-    <col min="10" max="10" width="6.6640625" style="179" customWidth="1"/>
+    <col min="10" max="10" width="6.6640625" style="166" customWidth="1"/>
     <col min="11" max="22" width="5.33203125" style="1" customWidth="1"/>
     <col min="23" max="23" width="5.33203125" style="2" customWidth="1"/>
     <col min="24" max="24" width="5.6640625" style="2"/>
@@ -45166,29 +45163,29 @@
   <sheetData>
     <row r="1" spans="1:23" ht="0.75" customHeight="1"/>
     <row r="2" spans="1:23" ht="12.75" customHeight="1">
-      <c r="A2" s="168"/>
-      <c r="B2" s="168"/>
-      <c r="C2" s="168"/>
-      <c r="D2" s="168"/>
-      <c r="E2" s="168"/>
-      <c r="F2" s="168"/>
-      <c r="G2" s="168"/>
-      <c r="H2" s="168"/>
-      <c r="I2" s="168"/>
-      <c r="J2" s="168"/>
-      <c r="K2" s="168"/>
-      <c r="L2" s="168"/>
-      <c r="M2" s="168"/>
-      <c r="N2" s="168"/>
-      <c r="O2" s="168"/>
-      <c r="P2" s="168"/>
-      <c r="Q2" s="168"/>
-      <c r="R2" s="168"/>
-      <c r="S2" s="168"/>
-      <c r="T2" s="168"/>
-      <c r="U2" s="168"/>
-      <c r="V2" s="168"/>
-      <c r="W2" s="168"/>
+      <c r="A2" s="181"/>
+      <c r="B2" s="181"/>
+      <c r="C2" s="181"/>
+      <c r="D2" s="181"/>
+      <c r="E2" s="181"/>
+      <c r="F2" s="181"/>
+      <c r="G2" s="181"/>
+      <c r="H2" s="181"/>
+      <c r="I2" s="181"/>
+      <c r="J2" s="181"/>
+      <c r="K2" s="181"/>
+      <c r="L2" s="181"/>
+      <c r="M2" s="181"/>
+      <c r="N2" s="181"/>
+      <c r="O2" s="181"/>
+      <c r="P2" s="181"/>
+      <c r="Q2" s="181"/>
+      <c r="R2" s="181"/>
+      <c r="S2" s="181"/>
+      <c r="T2" s="181"/>
+      <c r="U2" s="181"/>
+      <c r="V2" s="181"/>
+      <c r="W2" s="181"/>
     </row>
     <row r="3" spans="1:23" ht="0.75" customHeight="1" thickBot="1">
       <c r="A3" s="3"/>
@@ -45220,13 +45217,13 @@
       <c r="B4" s="4"/>
       <c r="C4" s="5"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="169"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="170"/>
-      <c r="K4" s="180"/>
+      <c r="E4" s="182"/>
+      <c r="F4" s="183"/>
+      <c r="G4" s="183"/>
+      <c r="H4" s="183"/>
+      <c r="I4" s="184"/>
+      <c r="J4" s="185"/>
+      <c r="K4" s="183"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
@@ -45266,33 +45263,33 @@
       <c r="W5" s="14"/>
     </row>
     <row r="6" spans="1:23" ht="12.75" customHeight="1" thickBot="1">
-      <c r="A6" s="171"/>
-      <c r="B6" s="171"/>
-      <c r="C6" s="171"/>
-      <c r="D6" s="171"/>
-      <c r="E6" s="171"/>
-      <c r="F6" s="171"/>
-      <c r="G6" s="171"/>
-      <c r="H6" s="171"/>
-      <c r="I6" s="171"/>
-      <c r="J6" s="171"/>
-      <c r="K6" s="171"/>
-      <c r="L6" s="171"/>
-      <c r="M6" s="171"/>
-      <c r="N6" s="171"/>
-      <c r="O6" s="171"/>
-      <c r="P6" s="171"/>
-      <c r="Q6" s="171"/>
-      <c r="R6" s="171"/>
-      <c r="S6" s="171"/>
-      <c r="T6" s="171"/>
-      <c r="U6" s="171"/>
-      <c r="V6" s="171"/>
-      <c r="W6" s="171"/>
+      <c r="A6" s="186"/>
+      <c r="B6" s="186"/>
+      <c r="C6" s="186"/>
+      <c r="D6" s="186"/>
+      <c r="E6" s="186"/>
+      <c r="F6" s="186"/>
+      <c r="G6" s="186"/>
+      <c r="H6" s="186"/>
+      <c r="I6" s="186"/>
+      <c r="J6" s="186"/>
+      <c r="K6" s="186"/>
+      <c r="L6" s="186"/>
+      <c r="M6" s="186"/>
+      <c r="N6" s="186"/>
+      <c r="O6" s="186"/>
+      <c r="P6" s="186"/>
+      <c r="Q6" s="186"/>
+      <c r="R6" s="186"/>
+      <c r="S6" s="186"/>
+      <c r="T6" s="186"/>
+      <c r="U6" s="186"/>
+      <c r="V6" s="186"/>
+      <c r="W6" s="186"/>
     </row>
     <row r="7" spans="1:23" ht="12" customHeight="1">
-      <c r="A7" s="172"/>
-      <c r="B7" s="173"/>
+      <c r="A7" s="187"/>
+      <c r="B7" s="188"/>
       <c r="C7" s="15"/>
       <c r="D7" s="16"/>
       <c r="E7" s="139"/>
@@ -45316,8 +45313,8 @@
       <c r="W7" s="21"/>
     </row>
     <row r="8" spans="1:23" ht="12" customHeight="1">
-      <c r="A8" s="174"/>
-      <c r="B8" s="175"/>
+      <c r="A8" s="177"/>
+      <c r="B8" s="178"/>
       <c r="C8" s="22"/>
       <c r="D8" s="23"/>
       <c r="E8" s="140"/>
@@ -45341,8 +45338,8 @@
       <c r="W8" s="30"/>
     </row>
     <row r="9" spans="1:23" ht="12" customHeight="1">
-      <c r="A9" s="176"/>
-      <c r="B9" s="177"/>
+      <c r="A9" s="179"/>
+      <c r="B9" s="180"/>
       <c r="C9" s="22"/>
       <c r="D9" s="31"/>
       <c r="E9" s="32"/>
@@ -45366,8 +45363,8 @@
       <c r="W9" s="40"/>
     </row>
     <row r="10" spans="1:23" ht="12" customHeight="1">
-      <c r="A10" s="174"/>
-      <c r="B10" s="175"/>
+      <c r="A10" s="177"/>
+      <c r="B10" s="178"/>
       <c r="C10" s="22"/>
       <c r="D10" s="41"/>
       <c r="E10" s="24"/>
@@ -45391,14 +45388,14 @@
       <c r="W10" s="30"/>
     </row>
     <row r="11" spans="1:23" ht="12" customHeight="1">
-      <c r="A11" s="174"/>
-      <c r="B11" s="175"/>
+      <c r="A11" s="177"/>
+      <c r="B11" s="178"/>
       <c r="C11" s="22"/>
       <c r="D11" s="23"/>
       <c r="E11" s="43"/>
-      <c r="F11" s="182"/>
+      <c r="F11" s="167"/>
       <c r="G11" s="2"/>
-      <c r="H11" s="183"/>
+      <c r="H11" s="168"/>
       <c r="I11" s="25"/>
       <c r="J11" s="44"/>
       <c r="K11" s="45"/>
@@ -45416,14 +45413,14 @@
       <c r="W11" s="47"/>
     </row>
     <row r="12" spans="1:23" ht="12" customHeight="1">
-      <c r="A12" s="162"/>
-      <c r="B12" s="162"/>
+      <c r="A12" s="161"/>
+      <c r="B12" s="161"/>
       <c r="C12" s="48"/>
       <c r="D12" s="23"/>
       <c r="E12" s="24"/>
-      <c r="F12" s="182"/>
+      <c r="F12" s="167"/>
       <c r="G12" s="2"/>
-      <c r="H12" s="183"/>
+      <c r="H12" s="168"/>
       <c r="I12" s="25"/>
       <c r="J12" s="49"/>
       <c r="K12" s="50"/>
@@ -45441,10 +45438,10 @@
       <c r="W12" s="52"/>
     </row>
     <row r="13" spans="1:23" ht="12" customHeight="1">
-      <c r="A13" s="162"/>
-      <c r="B13" s="162"/>
-      <c r="C13" s="167"/>
-      <c r="D13" s="184"/>
+      <c r="A13" s="161"/>
+      <c r="B13" s="161"/>
+      <c r="C13" s="173"/>
+      <c r="D13" s="174"/>
       <c r="E13" s="141"/>
       <c r="F13" s="142"/>
       <c r="G13" s="142"/>
@@ -45493,8 +45490,8 @@
     <row r="15" spans="1:23" ht="12" customHeight="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="178"/>
-      <c r="D15" s="185"/>
+      <c r="C15" s="175"/>
+      <c r="D15" s="176"/>
       <c r="E15" s="143"/>
       <c r="F15" s="67"/>
       <c r="G15" s="67"/>
@@ -45518,8 +45515,8 @@
     <row r="16" spans="1:23" ht="12" customHeight="1">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="167"/>
-      <c r="D16" s="184"/>
+      <c r="C16" s="173"/>
+      <c r="D16" s="174"/>
       <c r="E16" s="141"/>
       <c r="F16" s="142"/>
       <c r="G16" s="142"/>
@@ -45566,10 +45563,10 @@
       <c r="W17" s="77"/>
     </row>
     <row r="18" spans="1:23" ht="12" customHeight="1">
-      <c r="A18" s="162"/>
-      <c r="B18" s="162"/>
-      <c r="C18" s="167"/>
-      <c r="D18" s="184"/>
+      <c r="A18" s="161"/>
+      <c r="B18" s="161"/>
+      <c r="C18" s="173"/>
+      <c r="D18" s="174"/>
       <c r="E18" s="78"/>
       <c r="F18" s="68"/>
       <c r="G18" s="68"/>
@@ -45591,10 +45588,10 @@
       <c r="W18" s="74"/>
     </row>
     <row r="19" spans="1:23" ht="12" customHeight="1">
-      <c r="A19" s="162"/>
-      <c r="B19" s="162"/>
+      <c r="A19" s="161"/>
+      <c r="B19" s="161"/>
       <c r="C19" s="80"/>
-      <c r="D19" s="163"/>
+      <c r="D19" s="162"/>
       <c r="E19" s="81"/>
       <c r="F19" s="82"/>
       <c r="G19" s="83"/>
@@ -45616,10 +45613,10 @@
       <c r="W19" s="40"/>
     </row>
     <row r="20" spans="1:23" ht="12" customHeight="1">
-      <c r="A20" s="162"/>
-      <c r="B20" s="162"/>
+      <c r="A20" s="161"/>
+      <c r="B20" s="161"/>
       <c r="C20" s="80"/>
-      <c r="D20" s="163"/>
+      <c r="D20" s="162"/>
       <c r="E20" s="81"/>
       <c r="F20" s="82"/>
       <c r="G20" s="83"/>
@@ -45641,8 +45638,8 @@
       <c r="W20" s="30"/>
     </row>
     <row r="21" spans="1:23" ht="12" customHeight="1">
-      <c r="A21" s="162"/>
-      <c r="B21" s="162"/>
+      <c r="A21" s="161"/>
+      <c r="B21" s="161"/>
       <c r="C21" s="58"/>
       <c r="D21" s="59"/>
       <c r="E21" s="90"/>
@@ -45666,10 +45663,10 @@
       <c r="W21" s="77"/>
     </row>
     <row r="22" spans="1:23" ht="12" customHeight="1">
-      <c r="A22" s="162"/>
-      <c r="B22" s="162"/>
-      <c r="C22" s="167"/>
-      <c r="D22" s="184"/>
+      <c r="A22" s="161"/>
+      <c r="B22" s="161"/>
+      <c r="C22" s="173"/>
+      <c r="D22" s="174"/>
       <c r="E22" s="78"/>
       <c r="F22" s="68"/>
       <c r="G22" s="68"/>
@@ -45691,10 +45688,10 @@
       <c r="W22" s="74"/>
     </row>
     <row r="23" spans="1:23" ht="12" customHeight="1">
-      <c r="A23" s="162"/>
-      <c r="B23" s="162"/>
+      <c r="A23" s="161"/>
+      <c r="B23" s="161"/>
       <c r="C23" s="80"/>
-      <c r="D23" s="163"/>
+      <c r="D23" s="162"/>
       <c r="E23" s="81"/>
       <c r="F23" s="82"/>
       <c r="G23" s="83"/>
@@ -45716,10 +45713,10 @@
       <c r="W23" s="40"/>
     </row>
     <row r="24" spans="1:23" ht="12" customHeight="1">
-      <c r="A24" s="162"/>
-      <c r="B24" s="162"/>
+      <c r="A24" s="161"/>
+      <c r="B24" s="161"/>
       <c r="C24" s="80"/>
-      <c r="D24" s="163"/>
+      <c r="D24" s="162"/>
       <c r="E24" s="81"/>
       <c r="F24" s="82"/>
       <c r="G24" s="83"/>
@@ -45741,8 +45738,8 @@
       <c r="W24" s="30"/>
     </row>
     <row r="25" spans="1:23" ht="12" customHeight="1">
-      <c r="A25" s="162"/>
-      <c r="B25" s="162"/>
+      <c r="A25" s="161"/>
+      <c r="B25" s="161"/>
       <c r="C25" s="58"/>
       <c r="D25" s="59"/>
       <c r="E25" s="90"/>
@@ -45766,10 +45763,10 @@
       <c r="W25" s="77"/>
     </row>
     <row r="26" spans="1:23" ht="12" customHeight="1">
-      <c r="A26" s="162"/>
-      <c r="B26" s="162"/>
-      <c r="C26" s="167"/>
-      <c r="D26" s="184"/>
+      <c r="A26" s="161"/>
+      <c r="B26" s="161"/>
+      <c r="C26" s="173"/>
+      <c r="D26" s="174"/>
       <c r="E26" s="78"/>
       <c r="F26" s="68"/>
       <c r="G26" s="68"/>
@@ -45791,10 +45788,10 @@
       <c r="W26" s="74"/>
     </row>
     <row r="27" spans="1:23" ht="12" customHeight="1">
-      <c r="A27" s="162"/>
-      <c r="B27" s="162"/>
+      <c r="A27" s="161"/>
+      <c r="B27" s="161"/>
       <c r="C27" s="80"/>
-      <c r="D27" s="163"/>
+      <c r="D27" s="162"/>
       <c r="E27" s="81"/>
       <c r="F27" s="82"/>
       <c r="G27" s="83"/>
@@ -45816,10 +45813,10 @@
       <c r="W27" s="40"/>
     </row>
     <row r="28" spans="1:23" ht="12" customHeight="1">
-      <c r="A28" s="162"/>
-      <c r="B28" s="162"/>
+      <c r="A28" s="161"/>
+      <c r="B28" s="161"/>
       <c r="C28" s="80"/>
-      <c r="D28" s="163"/>
+      <c r="D28" s="162"/>
       <c r="E28" s="81"/>
       <c r="F28" s="82"/>
       <c r="G28" s="83"/>
@@ -45841,8 +45838,8 @@
       <c r="W28" s="30"/>
     </row>
     <row r="29" spans="1:23" ht="12" customHeight="1">
-      <c r="A29" s="162"/>
-      <c r="B29" s="162"/>
+      <c r="A29" s="161"/>
+      <c r="B29" s="161"/>
       <c r="C29" s="58"/>
       <c r="D29" s="59"/>
       <c r="E29" s="90"/>
@@ -45866,10 +45863,10 @@
       <c r="W29" s="77"/>
     </row>
     <row r="30" spans="1:23" ht="12" customHeight="1">
-      <c r="A30" s="162"/>
-      <c r="B30" s="162"/>
-      <c r="C30" s="167"/>
-      <c r="D30" s="184"/>
+      <c r="A30" s="161"/>
+      <c r="B30" s="161"/>
+      <c r="C30" s="173"/>
+      <c r="D30" s="174"/>
       <c r="E30" s="148"/>
       <c r="F30" s="68"/>
       <c r="G30" s="68"/>
@@ -45891,10 +45888,10 @@
       <c r="W30" s="74"/>
     </row>
     <row r="31" spans="1:23" ht="12" customHeight="1">
-      <c r="A31" s="162"/>
-      <c r="B31" s="162"/>
+      <c r="A31" s="161"/>
+      <c r="B31" s="161"/>
       <c r="C31" s="80"/>
-      <c r="D31" s="163"/>
+      <c r="D31" s="162"/>
       <c r="E31" s="149"/>
       <c r="F31" s="83"/>
       <c r="G31" s="83"/>
@@ -45916,10 +45913,10 @@
       <c r="W31" s="40"/>
     </row>
     <row r="32" spans="1:23" ht="12" customHeight="1">
-      <c r="A32" s="162"/>
-      <c r="B32" s="162"/>
+      <c r="A32" s="161"/>
+      <c r="B32" s="161"/>
       <c r="C32" s="80"/>
-      <c r="D32" s="163"/>
+      <c r="D32" s="162"/>
       <c r="E32" s="149"/>
       <c r="F32" s="83"/>
       <c r="G32" s="83"/>
@@ -45941,8 +45938,8 @@
       <c r="W32" s="30"/>
     </row>
     <row r="33" spans="1:23" ht="12" customHeight="1">
-      <c r="A33" s="162"/>
-      <c r="B33" s="162"/>
+      <c r="A33" s="161"/>
+      <c r="B33" s="161"/>
       <c r="C33" s="58"/>
       <c r="D33" s="59"/>
       <c r="E33" s="150"/>
@@ -45966,10 +45963,10 @@
       <c r="W33" s="77"/>
     </row>
     <row r="34" spans="1:23" ht="12" customHeight="1">
-      <c r="A34" s="162"/>
-      <c r="B34" s="162"/>
-      <c r="C34" s="167"/>
-      <c r="D34" s="184"/>
+      <c r="A34" s="161"/>
+      <c r="B34" s="161"/>
+      <c r="C34" s="173"/>
+      <c r="D34" s="174"/>
       <c r="E34" s="99"/>
       <c r="F34" s="100"/>
       <c r="G34" s="79"/>
@@ -45991,10 +45988,10 @@
       <c r="W34" s="105"/>
     </row>
     <row r="35" spans="1:23" ht="12" customHeight="1">
-      <c r="A35" s="162"/>
-      <c r="B35" s="162"/>
+      <c r="A35" s="161"/>
+      <c r="B35" s="161"/>
       <c r="C35" s="80"/>
-      <c r="D35" s="163"/>
+      <c r="D35" s="162"/>
       <c r="E35" s="96"/>
       <c r="F35" s="87"/>
       <c r="G35" s="87"/>
@@ -46016,10 +46013,10 @@
       <c r="W35" s="110"/>
     </row>
     <row r="36" spans="1:23" ht="12" customHeight="1">
-      <c r="A36" s="162"/>
-      <c r="B36" s="162"/>
+      <c r="A36" s="161"/>
+      <c r="B36" s="161"/>
       <c r="C36" s="80"/>
-      <c r="D36" s="163"/>
+      <c r="D36" s="162"/>
       <c r="E36" s="149"/>
       <c r="F36" s="83"/>
       <c r="G36" s="83"/>
@@ -46041,8 +46038,8 @@
       <c r="W36" s="30"/>
     </row>
     <row r="37" spans="1:23" ht="12" customHeight="1">
-      <c r="A37" s="162"/>
-      <c r="B37" s="162"/>
+      <c r="A37" s="161"/>
+      <c r="B37" s="161"/>
       <c r="C37" s="58"/>
       <c r="D37" s="59"/>
       <c r="E37" s="150"/>
@@ -46066,10 +46063,10 @@
       <c r="W37" s="113"/>
     </row>
     <row r="38" spans="1:23" ht="12" customHeight="1">
-      <c r="A38" s="162"/>
-      <c r="B38" s="162"/>
-      <c r="C38" s="167"/>
-      <c r="D38" s="184"/>
+      <c r="A38" s="161"/>
+      <c r="B38" s="161"/>
+      <c r="C38" s="173"/>
+      <c r="D38" s="174"/>
       <c r="E38" s="151"/>
       <c r="F38" s="56"/>
       <c r="G38" s="56"/>
@@ -46091,10 +46088,10 @@
       <c r="W38" s="74"/>
     </row>
     <row r="39" spans="1:23" ht="12" customHeight="1">
-      <c r="A39" s="162"/>
-      <c r="B39" s="162"/>
+      <c r="A39" s="161"/>
+      <c r="B39" s="161"/>
       <c r="C39" s="80"/>
-      <c r="D39" s="163"/>
+      <c r="D39" s="162"/>
       <c r="E39" s="152"/>
       <c r="F39" s="122"/>
       <c r="G39" s="122"/>
@@ -46116,10 +46113,10 @@
       <c r="W39" s="40"/>
     </row>
     <row r="40" spans="1:23" ht="12" customHeight="1">
-      <c r="A40" s="162"/>
-      <c r="B40" s="162"/>
+      <c r="A40" s="161"/>
+      <c r="B40" s="161"/>
       <c r="C40" s="80"/>
-      <c r="D40" s="163"/>
+      <c r="D40" s="162"/>
       <c r="E40" s="149"/>
       <c r="F40" s="83"/>
       <c r="G40" s="83"/>
@@ -46141,8 +46138,8 @@
       <c r="W40" s="30"/>
     </row>
     <row r="41" spans="1:23" ht="12" customHeight="1">
-      <c r="A41" s="162"/>
-      <c r="B41" s="162"/>
+      <c r="A41" s="161"/>
+      <c r="B41" s="161"/>
       <c r="C41" s="58"/>
       <c r="D41" s="59"/>
       <c r="E41" s="150"/>
@@ -46166,10 +46163,10 @@
       <c r="W41" s="77"/>
     </row>
     <row r="42" spans="1:23" ht="12" customHeight="1">
-      <c r="A42" s="162"/>
-      <c r="B42" s="162"/>
-      <c r="C42" s="167"/>
-      <c r="D42" s="184"/>
+      <c r="A42" s="161"/>
+      <c r="B42" s="161"/>
+      <c r="C42" s="173"/>
+      <c r="D42" s="174"/>
       <c r="E42" s="151"/>
       <c r="F42" s="56"/>
       <c r="G42" s="56"/>
@@ -46191,10 +46188,10 @@
       <c r="W42" s="74"/>
     </row>
     <row r="43" spans="1:23" ht="12" customHeight="1">
-      <c r="A43" s="162"/>
-      <c r="B43" s="162"/>
+      <c r="A43" s="161"/>
+      <c r="B43" s="161"/>
       <c r="C43" s="80"/>
-      <c r="D43" s="163"/>
+      <c r="D43" s="162"/>
       <c r="E43" s="152"/>
       <c r="F43" s="122"/>
       <c r="G43" s="122"/>
@@ -46216,10 +46213,10 @@
       <c r="W43" s="40"/>
     </row>
     <row r="44" spans="1:23" ht="12" customHeight="1">
-      <c r="A44" s="162"/>
-      <c r="B44" s="162"/>
+      <c r="A44" s="161"/>
+      <c r="B44" s="161"/>
       <c r="C44" s="80"/>
-      <c r="D44" s="163"/>
+      <c r="D44" s="162"/>
       <c r="E44" s="149"/>
       <c r="F44" s="83"/>
       <c r="G44" s="83"/>
@@ -46241,8 +46238,8 @@
       <c r="W44" s="30"/>
     </row>
     <row r="45" spans="1:23" ht="12" customHeight="1">
-      <c r="A45" s="162"/>
-      <c r="B45" s="162"/>
+      <c r="A45" s="161"/>
+      <c r="B45" s="161"/>
       <c r="C45" s="58"/>
       <c r="D45" s="59"/>
       <c r="E45" s="150"/>
@@ -46266,10 +46263,10 @@
       <c r="W45" s="77"/>
     </row>
     <row r="46" spans="1:23" ht="12" customHeight="1">
-      <c r="A46" s="162"/>
-      <c r="B46" s="162"/>
-      <c r="C46" s="167"/>
-      <c r="D46" s="184"/>
+      <c r="A46" s="161"/>
+      <c r="B46" s="161"/>
+      <c r="C46" s="173"/>
+      <c r="D46" s="174"/>
       <c r="E46" s="78"/>
       <c r="F46" s="116"/>
       <c r="G46" s="56"/>
@@ -46291,10 +46288,10 @@
       <c r="W46" s="74"/>
     </row>
     <row r="47" spans="1:23" ht="12" customHeight="1">
-      <c r="A47" s="162"/>
-      <c r="B47" s="162"/>
+      <c r="A47" s="161"/>
+      <c r="B47" s="161"/>
       <c r="C47" s="80"/>
-      <c r="D47" s="163"/>
+      <c r="D47" s="162"/>
       <c r="E47" s="81"/>
       <c r="F47" s="51"/>
       <c r="G47" s="122"/>
@@ -46316,10 +46313,10 @@
       <c r="W47" s="40"/>
     </row>
     <row r="48" spans="1:23" ht="12" customHeight="1">
-      <c r="A48" s="162"/>
-      <c r="B48" s="162"/>
+      <c r="A48" s="161"/>
+      <c r="B48" s="161"/>
       <c r="C48" s="80"/>
-      <c r="D48" s="163"/>
+      <c r="D48" s="162"/>
       <c r="E48" s="81"/>
       <c r="F48" s="51"/>
       <c r="G48" s="117"/>
@@ -46341,8 +46338,8 @@
       <c r="W48" s="30"/>
     </row>
     <row r="49" spans="1:23" ht="12" customHeight="1">
-      <c r="A49" s="162"/>
-      <c r="B49" s="162"/>
+      <c r="A49" s="161"/>
+      <c r="B49" s="161"/>
       <c r="C49" s="58"/>
       <c r="D49" s="59"/>
       <c r="E49" s="90"/>
@@ -46366,10 +46363,10 @@
       <c r="W49" s="77"/>
     </row>
     <row r="50" spans="1:23" ht="12" customHeight="1">
-      <c r="A50" s="162"/>
-      <c r="B50" s="162"/>
-      <c r="C50" s="167"/>
-      <c r="D50" s="184"/>
+      <c r="A50" s="161"/>
+      <c r="B50" s="161"/>
+      <c r="C50" s="173"/>
+      <c r="D50" s="174"/>
       <c r="E50" s="78"/>
       <c r="F50" s="116"/>
       <c r="G50" s="56"/>
@@ -46391,10 +46388,10 @@
       <c r="W50" s="74"/>
     </row>
     <row r="51" spans="1:23" ht="12" customHeight="1">
-      <c r="A51" s="162"/>
-      <c r="B51" s="162"/>
+      <c r="A51" s="161"/>
+      <c r="B51" s="161"/>
       <c r="C51" s="80"/>
-      <c r="D51" s="163"/>
+      <c r="D51" s="162"/>
       <c r="E51" s="81"/>
       <c r="F51" s="51"/>
       <c r="G51" s="122"/>
@@ -46416,10 +46413,10 @@
       <c r="W51" s="40"/>
     </row>
     <row r="52" spans="1:23" ht="12" customHeight="1">
-      <c r="A52" s="162"/>
-      <c r="B52" s="162"/>
+      <c r="A52" s="161"/>
+      <c r="B52" s="161"/>
       <c r="C52" s="80"/>
-      <c r="D52" s="163"/>
+      <c r="D52" s="162"/>
       <c r="E52" s="81"/>
       <c r="F52" s="51"/>
       <c r="G52" s="117"/>
@@ -46441,8 +46438,8 @@
       <c r="W52" s="30"/>
     </row>
     <row r="53" spans="1:23" ht="12" customHeight="1">
-      <c r="A53" s="162"/>
-      <c r="B53" s="162"/>
+      <c r="A53" s="161"/>
+      <c r="B53" s="161"/>
       <c r="C53" s="58"/>
       <c r="D53" s="59"/>
       <c r="E53" s="90"/>
@@ -46466,14 +46463,14 @@
       <c r="W53" s="123"/>
     </row>
     <row r="55" spans="1:23" ht="12" customHeight="1">
-      <c r="C55" s="186"/>
+      <c r="C55" s="169"/>
       <c r="D55" s="124"/>
       <c r="E55" s="124"/>
       <c r="F55" s="124"/>
       <c r="G55" s="124"/>
       <c r="H55" s="124"/>
       <c r="I55" s="124"/>
-      <c r="J55" s="187"/>
+      <c r="J55" s="170"/>
       <c r="K55" s="124"/>
       <c r="L55" s="124"/>
       <c r="M55" s="124"/>
@@ -46489,14 +46486,14 @@
       <c r="W55" s="124"/>
     </row>
     <row r="56" spans="1:23" ht="12" customHeight="1">
-      <c r="C56" s="188"/>
+      <c r="C56" s="171"/>
       <c r="D56" s="125"/>
       <c r="E56" s="125"/>
       <c r="F56" s="125"/>
       <c r="G56" s="125"/>
       <c r="H56" s="125"/>
       <c r="I56" s="125"/>
-      <c r="J56" s="189"/>
+      <c r="J56" s="172"/>
       <c r="K56" s="125"/>
       <c r="L56" s="125"/>
       <c r="M56" s="125"/>
@@ -46512,14 +46509,14 @@
       <c r="W56" s="126"/>
     </row>
     <row r="57" spans="1:23" ht="12" customHeight="1">
-      <c r="C57" s="188"/>
+      <c r="C57" s="171"/>
       <c r="D57" s="125"/>
       <c r="E57" s="125"/>
       <c r="F57" s="125"/>
       <c r="G57" s="125"/>
       <c r="H57" s="125"/>
       <c r="I57" s="125"/>
-      <c r="J57" s="189"/>
+      <c r="J57" s="172"/>
       <c r="K57" s="125"/>
       <c r="L57" s="125"/>
       <c r="M57" s="125"/>
@@ -46535,14 +46532,14 @@
       <c r="W57" s="126"/>
     </row>
     <row r="58" spans="1:23" ht="12" customHeight="1">
-      <c r="C58" s="188"/>
+      <c r="C58" s="171"/>
       <c r="D58" s="125"/>
       <c r="E58" s="125"/>
       <c r="F58" s="125"/>
       <c r="G58" s="125"/>
       <c r="H58" s="125"/>
       <c r="I58" s="125"/>
-      <c r="J58" s="189"/>
+      <c r="J58" s="172"/>
       <c r="K58" s="125"/>
       <c r="L58" s="125"/>
       <c r="M58" s="125"/>
@@ -46558,14 +46555,14 @@
       <c r="W58" s="126"/>
     </row>
     <row r="59" spans="1:23" ht="12" customHeight="1">
-      <c r="C59" s="188"/>
+      <c r="C59" s="171"/>
       <c r="D59" s="125"/>
       <c r="E59" s="125"/>
       <c r="F59" s="125"/>
       <c r="G59" s="125"/>
       <c r="H59" s="125"/>
       <c r="I59" s="125"/>
-      <c r="J59" s="189"/>
+      <c r="J59" s="172"/>
       <c r="K59" s="125"/>
       <c r="L59" s="125"/>
       <c r="M59" s="125"/>
@@ -46581,14 +46578,14 @@
       <c r="W59" s="126"/>
     </row>
     <row r="60" spans="1:23" ht="12" customHeight="1">
-      <c r="C60" s="188"/>
+      <c r="C60" s="171"/>
       <c r="D60" s="125"/>
       <c r="E60" s="125"/>
       <c r="F60" s="125"/>
       <c r="G60" s="125"/>
       <c r="H60" s="125"/>
       <c r="I60" s="125"/>
-      <c r="J60" s="189"/>
+      <c r="J60" s="172"/>
       <c r="K60" s="125"/>
       <c r="L60" s="125"/>
       <c r="M60" s="125"/>
@@ -46604,14 +46601,14 @@
       <c r="W60" s="126"/>
     </row>
     <row r="61" spans="1:23" ht="12" customHeight="1">
-      <c r="C61" s="188"/>
+      <c r="C61" s="171"/>
       <c r="D61" s="125"/>
       <c r="E61" s="125"/>
       <c r="F61" s="125"/>
       <c r="G61" s="125"/>
       <c r="H61" s="125"/>
       <c r="I61" s="125"/>
-      <c r="J61" s="189"/>
+      <c r="J61" s="172"/>
       <c r="K61" s="125"/>
       <c r="L61" s="125"/>
       <c r="M61" s="125"/>
@@ -46627,8 +46624,8 @@
       <c r="W61" s="126"/>
     </row>
     <row r="64" spans="1:23" ht="12" customHeight="1">
-      <c r="C64" s="167"/>
-      <c r="D64" s="184"/>
+      <c r="C64" s="173"/>
+      <c r="D64" s="174"/>
       <c r="E64" s="141"/>
       <c r="F64" s="142"/>
       <c r="G64" s="142"/>
@@ -46673,10 +46670,10 @@
       <c r="W65" s="30"/>
     </row>
     <row r="66" spans="1:23" ht="12" customHeight="1">
-      <c r="A66" s="162"/>
-      <c r="B66" s="162"/>
-      <c r="C66" s="167"/>
-      <c r="D66" s="184"/>
+      <c r="A66" s="161"/>
+      <c r="B66" s="161"/>
+      <c r="C66" s="173"/>
+      <c r="D66" s="174"/>
       <c r="E66" s="78"/>
       <c r="F66" s="68"/>
       <c r="G66" s="68"/>
@@ -46698,10 +46695,10 @@
       <c r="W66" s="57"/>
     </row>
     <row r="67" spans="1:23" ht="12" customHeight="1">
-      <c r="A67" s="162"/>
-      <c r="B67" s="162"/>
+      <c r="A67" s="161"/>
+      <c r="B67" s="161"/>
       <c r="C67" s="80"/>
-      <c r="D67" s="163"/>
+      <c r="D67" s="162"/>
       <c r="E67" s="81"/>
       <c r="F67" s="82"/>
       <c r="G67" s="83"/>
@@ -46723,10 +46720,10 @@
       <c r="W67" s="30"/>
     </row>
     <row r="68" spans="1:23" ht="12" customHeight="1">
-      <c r="A68" s="162"/>
-      <c r="B68" s="162"/>
+      <c r="A68" s="161"/>
+      <c r="B68" s="161"/>
       <c r="C68" s="80"/>
-      <c r="D68" s="163"/>
+      <c r="D68" s="162"/>
       <c r="E68" s="81"/>
       <c r="F68" s="82"/>
       <c r="G68" s="83"/>
@@ -46748,8 +46745,8 @@
       <c r="W68" s="77"/>
     </row>
     <row r="69" spans="1:23" ht="12" customHeight="1">
-      <c r="A69" s="162"/>
-      <c r="B69" s="162"/>
+      <c r="A69" s="161"/>
+      <c r="B69" s="161"/>
       <c r="C69" s="58"/>
       <c r="D69" s="59"/>
       <c r="E69" s="90"/>
@@ -46773,10 +46770,10 @@
       <c r="W69" s="30"/>
     </row>
     <row r="70" spans="1:23" ht="12" customHeight="1">
-      <c r="A70" s="162"/>
-      <c r="B70" s="162"/>
-      <c r="C70" s="167"/>
-      <c r="D70" s="184"/>
+      <c r="A70" s="161"/>
+      <c r="B70" s="161"/>
+      <c r="C70" s="173"/>
+      <c r="D70" s="174"/>
       <c r="E70" s="78"/>
       <c r="F70" s="68"/>
       <c r="G70" s="68"/>
@@ -46798,10 +46795,10 @@
       <c r="W70" s="57"/>
     </row>
     <row r="71" spans="1:23" ht="12" customHeight="1">
-      <c r="A71" s="162"/>
-      <c r="B71" s="162"/>
+      <c r="A71" s="161"/>
+      <c r="B71" s="161"/>
       <c r="C71" s="80"/>
-      <c r="D71" s="163"/>
+      <c r="D71" s="162"/>
       <c r="E71" s="81"/>
       <c r="F71" s="82"/>
       <c r="G71" s="83"/>
@@ -46823,10 +46820,10 @@
       <c r="W71" s="130"/>
     </row>
     <row r="72" spans="1:23" ht="12" customHeight="1">
-      <c r="A72" s="162"/>
-      <c r="B72" s="162"/>
+      <c r="A72" s="161"/>
+      <c r="B72" s="161"/>
       <c r="C72" s="80"/>
-      <c r="D72" s="163"/>
+      <c r="D72" s="162"/>
       <c r="E72" s="81"/>
       <c r="F72" s="82"/>
       <c r="G72" s="83"/>
@@ -46848,8 +46845,8 @@
       <c r="W72" s="77"/>
     </row>
     <row r="73" spans="1:23" ht="12" customHeight="1">
-      <c r="A73" s="162"/>
-      <c r="B73" s="162"/>
+      <c r="A73" s="161"/>
+      <c r="B73" s="161"/>
       <c r="C73" s="58"/>
       <c r="D73" s="59"/>
       <c r="E73" s="90"/>
@@ -46873,10 +46870,10 @@
       <c r="W73" s="30"/>
     </row>
     <row r="74" spans="1:23" ht="12" customHeight="1">
-      <c r="A74" s="162"/>
-      <c r="B74" s="162"/>
-      <c r="C74" s="167"/>
-      <c r="D74" s="184"/>
+      <c r="A74" s="161"/>
+      <c r="B74" s="161"/>
+      <c r="C74" s="173"/>
+      <c r="D74" s="174"/>
       <c r="E74" s="148"/>
       <c r="F74" s="68"/>
       <c r="G74" s="68"/>
@@ -46898,10 +46895,10 @@
       <c r="W74" s="57"/>
     </row>
     <row r="75" spans="1:23" ht="12" customHeight="1">
-      <c r="A75" s="162"/>
-      <c r="B75" s="162"/>
+      <c r="A75" s="161"/>
+      <c r="B75" s="161"/>
       <c r="C75" s="80"/>
-      <c r="D75" s="163"/>
+      <c r="D75" s="162"/>
       <c r="E75" s="149"/>
       <c r="F75" s="83"/>
       <c r="G75" s="83"/>
@@ -46923,10 +46920,10 @@
       <c r="W75" s="30"/>
     </row>
     <row r="76" spans="1:23" ht="12" customHeight="1">
-      <c r="A76" s="162"/>
-      <c r="B76" s="162"/>
+      <c r="A76" s="161"/>
+      <c r="B76" s="161"/>
       <c r="C76" s="80"/>
-      <c r="D76" s="163"/>
+      <c r="D76" s="162"/>
       <c r="E76" s="149"/>
       <c r="F76" s="83"/>
       <c r="G76" s="83"/>
@@ -46948,8 +46945,8 @@
       <c r="W76" s="77"/>
     </row>
     <row r="77" spans="1:23" ht="12" customHeight="1">
-      <c r="A77" s="162"/>
-      <c r="B77" s="162"/>
+      <c r="A77" s="161"/>
+      <c r="B77" s="161"/>
       <c r="C77" s="58"/>
       <c r="D77" s="59"/>
       <c r="E77" s="150"/>
@@ -46973,10 +46970,10 @@
       <c r="W77" s="30"/>
     </row>
     <row r="78" spans="1:23" ht="12" customHeight="1">
-      <c r="A78" s="162"/>
-      <c r="B78" s="162"/>
-      <c r="C78" s="167"/>
-      <c r="D78" s="184"/>
+      <c r="A78" s="161"/>
+      <c r="B78" s="161"/>
+      <c r="C78" s="173"/>
+      <c r="D78" s="174"/>
       <c r="E78" s="99"/>
       <c r="F78" s="100"/>
       <c r="G78" s="79"/>
@@ -46998,10 +46995,10 @@
       <c r="W78" s="105"/>
     </row>
     <row r="79" spans="1:23" ht="12" customHeight="1">
-      <c r="A79" s="162"/>
-      <c r="B79" s="162"/>
+      <c r="A79" s="161"/>
+      <c r="B79" s="161"/>
       <c r="C79" s="80"/>
-      <c r="D79" s="163"/>
+      <c r="D79" s="162"/>
       <c r="E79" s="149"/>
       <c r="F79" s="83"/>
       <c r="G79" s="83"/>
@@ -47023,10 +47020,10 @@
       <c r="W79" s="110"/>
     </row>
     <row r="80" spans="1:23" ht="12" customHeight="1">
-      <c r="A80" s="162"/>
-      <c r="B80" s="162"/>
+      <c r="A80" s="161"/>
+      <c r="B80" s="161"/>
       <c r="C80" s="80"/>
-      <c r="D80" s="163"/>
+      <c r="D80" s="162"/>
       <c r="E80" s="149"/>
       <c r="F80" s="83"/>
       <c r="G80" s="83"/>
@@ -47048,8 +47045,8 @@
       <c r="W80" s="77"/>
     </row>
     <row r="81" spans="1:23" ht="12" customHeight="1">
-      <c r="A81" s="162"/>
-      <c r="B81" s="162"/>
+      <c r="A81" s="161"/>
+      <c r="B81" s="161"/>
       <c r="C81" s="58"/>
       <c r="D81" s="59"/>
       <c r="E81" s="150"/>
@@ -47073,10 +47070,10 @@
       <c r="W81" s="113"/>
     </row>
     <row r="82" spans="1:23" ht="12" customHeight="1">
-      <c r="A82" s="162"/>
-      <c r="B82" s="162"/>
-      <c r="C82" s="167"/>
-      <c r="D82" s="184"/>
+      <c r="A82" s="161"/>
+      <c r="B82" s="161"/>
+      <c r="C82" s="173"/>
+      <c r="D82" s="174"/>
       <c r="E82" s="151"/>
       <c r="F82" s="56"/>
       <c r="G82" s="56"/>
@@ -47098,10 +47095,10 @@
       <c r="W82" s="57"/>
     </row>
     <row r="83" spans="1:23" ht="12" customHeight="1">
-      <c r="A83" s="162"/>
-      <c r="B83" s="162"/>
+      <c r="A83" s="161"/>
+      <c r="B83" s="161"/>
       <c r="C83" s="80"/>
-      <c r="D83" s="163"/>
+      <c r="D83" s="162"/>
       <c r="E83" s="152"/>
       <c r="F83" s="122"/>
       <c r="G83" s="122"/>
@@ -47123,10 +47120,10 @@
       <c r="W83" s="30"/>
     </row>
     <row r="84" spans="1:23" ht="12" customHeight="1">
-      <c r="A84" s="162"/>
-      <c r="B84" s="162"/>
+      <c r="A84" s="161"/>
+      <c r="B84" s="161"/>
       <c r="C84" s="80"/>
-      <c r="D84" s="163"/>
+      <c r="D84" s="162"/>
       <c r="E84" s="149"/>
       <c r="F84" s="83"/>
       <c r="G84" s="83"/>
@@ -47148,8 +47145,8 @@
       <c r="W84" s="77"/>
     </row>
     <row r="85" spans="1:23" ht="12" customHeight="1">
-      <c r="A85" s="162"/>
-      <c r="B85" s="162"/>
+      <c r="A85" s="161"/>
+      <c r="B85" s="161"/>
       <c r="C85" s="58"/>
       <c r="D85" s="59"/>
       <c r="E85" s="150"/>
@@ -47173,10 +47170,10 @@
       <c r="W85" s="30"/>
     </row>
     <row r="86" spans="1:23" ht="12" customHeight="1">
-      <c r="A86" s="162"/>
-      <c r="B86" s="162"/>
-      <c r="C86" s="167"/>
-      <c r="D86" s="184"/>
+      <c r="A86" s="161"/>
+      <c r="B86" s="161"/>
+      <c r="C86" s="173"/>
+      <c r="D86" s="174"/>
       <c r="E86" s="151"/>
       <c r="F86" s="56"/>
       <c r="G86" s="56"/>
@@ -47198,10 +47195,10 @@
       <c r="W86" s="57"/>
     </row>
     <row r="87" spans="1:23" ht="12" customHeight="1">
-      <c r="A87" s="162"/>
-      <c r="B87" s="162"/>
+      <c r="A87" s="161"/>
+      <c r="B87" s="161"/>
       <c r="C87" s="80"/>
-      <c r="D87" s="163"/>
+      <c r="D87" s="162"/>
       <c r="E87" s="152"/>
       <c r="F87" s="122"/>
       <c r="G87" s="122"/>
@@ -47223,10 +47220,10 @@
       <c r="W87" s="30"/>
     </row>
     <row r="88" spans="1:23" ht="12" customHeight="1">
-      <c r="A88" s="162"/>
-      <c r="B88" s="162"/>
+      <c r="A88" s="161"/>
+      <c r="B88" s="161"/>
       <c r="C88" s="80"/>
-      <c r="D88" s="163"/>
+      <c r="D88" s="162"/>
       <c r="E88" s="149"/>
       <c r="F88" s="83"/>
       <c r="G88" s="83"/>
@@ -47248,8 +47245,8 @@
       <c r="W88" s="77"/>
     </row>
     <row r="89" spans="1:23" ht="12" customHeight="1">
-      <c r="A89" s="162"/>
-      <c r="B89" s="162"/>
+      <c r="A89" s="161"/>
+      <c r="B89" s="161"/>
       <c r="C89" s="58"/>
       <c r="D89" s="59"/>
       <c r="E89" s="150"/>
@@ -47273,10 +47270,10 @@
       <c r="W89" s="30"/>
     </row>
     <row r="90" spans="1:23" ht="12" customHeight="1">
-      <c r="A90" s="162"/>
-      <c r="B90" s="162"/>
-      <c r="C90" s="167"/>
-      <c r="D90" s="184"/>
+      <c r="A90" s="161"/>
+      <c r="B90" s="161"/>
+      <c r="C90" s="173"/>
+      <c r="D90" s="174"/>
       <c r="E90" s="78"/>
       <c r="F90" s="116"/>
       <c r="G90" s="56"/>
@@ -47298,10 +47295,10 @@
       <c r="W90" s="57"/>
     </row>
     <row r="91" spans="1:23" ht="12" customHeight="1">
-      <c r="A91" s="162"/>
-      <c r="B91" s="162"/>
+      <c r="A91" s="161"/>
+      <c r="B91" s="161"/>
       <c r="C91" s="80"/>
-      <c r="D91" s="163"/>
+      <c r="D91" s="162"/>
       <c r="E91" s="81"/>
       <c r="F91" s="51"/>
       <c r="G91" s="122"/>
@@ -47323,10 +47320,10 @@
       <c r="W91" s="30"/>
     </row>
     <row r="92" spans="1:23" ht="12" customHeight="1">
-      <c r="A92" s="162"/>
-      <c r="B92" s="162"/>
+      <c r="A92" s="161"/>
+      <c r="B92" s="161"/>
       <c r="C92" s="80"/>
-      <c r="D92" s="163"/>
+      <c r="D92" s="162"/>
       <c r="E92" s="81"/>
       <c r="F92" s="51"/>
       <c r="G92" s="117"/>
@@ -47348,8 +47345,8 @@
       <c r="W92" s="77"/>
     </row>
     <row r="93" spans="1:23" ht="12" customHeight="1">
-      <c r="A93" s="162"/>
-      <c r="B93" s="162"/>
+      <c r="A93" s="161"/>
+      <c r="B93" s="161"/>
       <c r="C93" s="58"/>
       <c r="D93" s="59"/>
       <c r="E93" s="90"/>
@@ -47373,10 +47370,10 @@
       <c r="W93" s="30"/>
     </row>
     <row r="94" spans="1:23" ht="12" customHeight="1">
-      <c r="A94" s="162"/>
-      <c r="B94" s="162"/>
-      <c r="C94" s="167"/>
-      <c r="D94" s="184"/>
+      <c r="A94" s="161"/>
+      <c r="B94" s="161"/>
+      <c r="C94" s="173"/>
+      <c r="D94" s="174"/>
       <c r="E94" s="78"/>
       <c r="F94" s="116"/>
       <c r="G94" s="56"/>
@@ -47398,10 +47395,10 @@
       <c r="W94" s="137"/>
     </row>
     <row r="95" spans="1:23" ht="12" customHeight="1">
-      <c r="A95" s="162"/>
-      <c r="B95" s="162"/>
+      <c r="A95" s="161"/>
+      <c r="B95" s="161"/>
       <c r="C95" s="80"/>
-      <c r="D95" s="163"/>
+      <c r="D95" s="162"/>
       <c r="E95" s="81"/>
       <c r="F95" s="51"/>
       <c r="G95" s="122"/>
@@ -47423,10 +47420,10 @@
       <c r="W95" s="30"/>
     </row>
     <row r="96" spans="1:23" ht="12" customHeight="1">
-      <c r="A96" s="162"/>
-      <c r="B96" s="162"/>
+      <c r="A96" s="161"/>
+      <c r="B96" s="161"/>
       <c r="C96" s="80"/>
-      <c r="D96" s="163"/>
+      <c r="D96" s="162"/>
       <c r="E96" s="81"/>
       <c r="F96" s="51"/>
       <c r="G96" s="117"/>
@@ -47448,8 +47445,8 @@
       <c r="W96" s="77"/>
     </row>
     <row r="97" spans="1:23" ht="12" customHeight="1">
-      <c r="A97" s="162"/>
-      <c r="B97" s="163"/>
+      <c r="A97" s="161"/>
+      <c r="B97" s="162"/>
       <c r="C97" s="58"/>
       <c r="D97" s="59"/>
       <c r="E97" s="90"/>
@@ -47473,10 +47470,10 @@
       <c r="W97" s="138"/>
     </row>
     <row r="98" spans="1:23" ht="12" customHeight="1">
-      <c r="A98" s="162"/>
-      <c r="B98" s="162"/>
-      <c r="C98" s="167"/>
-      <c r="D98" s="184"/>
+      <c r="A98" s="161"/>
+      <c r="B98" s="161"/>
+      <c r="C98" s="173"/>
+      <c r="D98" s="174"/>
       <c r="E98" s="151"/>
       <c r="F98" s="56"/>
       <c r="G98" s="56"/>
@@ -47498,8 +47495,8 @@
       <c r="W98" s="74"/>
     </row>
     <row r="99" spans="1:23" ht="12" customHeight="1">
-      <c r="A99" s="162"/>
-      <c r="B99" s="162"/>
+      <c r="A99" s="161"/>
+      <c r="B99" s="161"/>
       <c r="C99" s="58"/>
       <c r="D99" s="59"/>
       <c r="E99" s="150"/>
@@ -47523,10 +47520,10 @@
       <c r="W99" s="123"/>
     </row>
     <row r="100" spans="1:23" ht="12" customHeight="1">
-      <c r="A100" s="162"/>
-      <c r="B100" s="162"/>
-      <c r="C100" s="167"/>
-      <c r="D100" s="184"/>
+      <c r="A100" s="161"/>
+      <c r="B100" s="161"/>
+      <c r="C100" s="173"/>
+      <c r="D100" s="174"/>
       <c r="E100" s="151"/>
       <c r="F100" s="56"/>
       <c r="G100" s="56"/>
@@ -47548,8 +47545,8 @@
       <c r="W100" s="137"/>
     </row>
     <row r="101" spans="1:23" ht="12" customHeight="1">
-      <c r="A101" s="162"/>
-      <c r="B101" s="162"/>
+      <c r="A101" s="161"/>
+      <c r="B101" s="161"/>
       <c r="C101" s="58"/>
       <c r="D101" s="59"/>
       <c r="E101" s="150"/>
@@ -47573,8 +47570,8 @@
       <c r="W101" s="138"/>
     </row>
     <row r="102" spans="1:23" ht="12" customHeight="1">
-      <c r="C102" s="167"/>
-      <c r="D102" s="184"/>
+      <c r="C102" s="173"/>
+      <c r="D102" s="174"/>
       <c r="E102" s="78"/>
       <c r="F102" s="116"/>
       <c r="G102" s="68"/>
@@ -47597,10 +47594,10 @@
     </row>
     <row r="103" spans="1:23" ht="12" customHeight="1">
       <c r="C103" s="80"/>
-      <c r="D103" s="163"/>
+      <c r="D103" s="162"/>
       <c r="E103" s="81"/>
       <c r="F103" s="51"/>
-      <c r="I103" s="166"/>
+      <c r="I103" s="165"/>
       <c r="J103" s="61"/>
       <c r="K103" s="42"/>
       <c r="L103" s="89"/>
@@ -47617,16 +47614,16 @@
       <c r="W103" s="30"/>
     </row>
     <row r="104" spans="1:23" ht="12" customHeight="1">
-      <c r="A104" s="162"/>
-      <c r="B104" s="162"/>
-      <c r="C104" s="167"/>
-      <c r="D104" s="184"/>
+      <c r="A104" s="161"/>
+      <c r="B104" s="161"/>
+      <c r="C104" s="173"/>
+      <c r="D104" s="174"/>
       <c r="E104" s="78"/>
       <c r="F104" s="116"/>
       <c r="G104" s="68"/>
       <c r="H104" s="68"/>
-      <c r="I104" s="165"/>
-      <c r="J104" s="161"/>
+      <c r="I104" s="164"/>
+      <c r="J104" s="71"/>
       <c r="K104" s="72"/>
       <c r="L104" s="73"/>
       <c r="M104" s="73"/>
@@ -47642,13 +47639,13 @@
       <c r="W104" s="74"/>
     </row>
     <row r="105" spans="1:23" ht="12" customHeight="1">
-      <c r="A105" s="162"/>
-      <c r="B105" s="162"/>
+      <c r="A105" s="161"/>
+      <c r="B105" s="161"/>
       <c r="C105" s="80"/>
-      <c r="D105" s="163"/>
+      <c r="D105" s="162"/>
       <c r="E105" s="81"/>
       <c r="F105" s="51"/>
-      <c r="I105" s="164"/>
+      <c r="I105" s="163"/>
       <c r="J105" s="85"/>
       <c r="K105" s="37"/>
       <c r="L105" s="86"/>
@@ -47666,6 +47663,24 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="C78:D78"/>
+    <mergeCell ref="C82:D82"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="C98:D98"/>
+    <mergeCell ref="C100:D100"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C90:D90"/>
+    <mergeCell ref="C94:D94"/>
+    <mergeCell ref="A2:W2"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A6:W6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C102:D102"/>
     <mergeCell ref="C104:D104"/>
     <mergeCell ref="C15:D15"/>
@@ -47682,24 +47697,6 @@
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C70:D70"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A2:W2"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A6:W6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C94:D94"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.98425196850393704" bottom="0.39370078740157483" header="0.39370078740157483" footer="0.31496062992125984"/>

</xml_diff>